<commit_message>
continued to add albums to list
</commit_message>
<xml_diff>
--- a/album_list.xlsx
+++ b/album_list.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP USER\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP USER\Coding\Play\Rap_Lyrics\lyricsNLP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68B5FCB5-1631-41E6-85AE-BFF960E836E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70C5E144-2482-4AF5-8DE5-BBCDADCF09A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4CD478C6-4722-4BC8-838A-CC153C60C18A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1707" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2669" uniqueCount="654">
   <si>
     <t>Artist</t>
   </si>
@@ -1305,6 +1305,699 @@
   </si>
   <si>
     <t>Queens</t>
+  </si>
+  <si>
+    <t>Megan Thee Stallion</t>
+  </si>
+  <si>
+    <t>Traumazine</t>
+  </si>
+  <si>
+    <t>Good News</t>
+  </si>
+  <si>
+    <t>City Girls</t>
+  </si>
+  <si>
+    <t>City on Lock</t>
+  </si>
+  <si>
+    <t>Girl Code</t>
+  </si>
+  <si>
+    <t>A Tribe Called Quest</t>
+  </si>
+  <si>
+    <t>We Got It from Here... Thank You 4 Your Service</t>
+  </si>
+  <si>
+    <t>People's Instinctive Travels and the Paths of Rhythm</t>
+  </si>
+  <si>
+    <t>The Low End Theory</t>
+  </si>
+  <si>
+    <t>Beats, Rhymes and Life</t>
+  </si>
+  <si>
+    <t>The Love Movement</t>
+  </si>
+  <si>
+    <t>Midnight Marauders</t>
+  </si>
+  <si>
+    <t>LL Cool J</t>
+  </si>
+  <si>
+    <t>Authentic</t>
+  </si>
+  <si>
+    <t>Radio</t>
+  </si>
+  <si>
+    <t>Bigger and Deffer</t>
+  </si>
+  <si>
+    <t>Walking with a Panther</t>
+  </si>
+  <si>
+    <t>Mama Said Knock You Out</t>
+  </si>
+  <si>
+    <t>14 Shots to the Dome</t>
+  </si>
+  <si>
+    <t>Mr. Smith</t>
+  </si>
+  <si>
+    <t>Phenomenon</t>
+  </si>
+  <si>
+    <t>G.O.A.T.</t>
+  </si>
+  <si>
+    <t>The DEFinition</t>
+  </si>
+  <si>
+    <t>Todd Smith</t>
+  </si>
+  <si>
+    <t>Exit 13</t>
+  </si>
+  <si>
+    <t>Run DMC</t>
+  </si>
+  <si>
+    <t>Crown Royal</t>
+  </si>
+  <si>
+    <t>Run-D.M.C.</t>
+  </si>
+  <si>
+    <t>King of Rock</t>
+  </si>
+  <si>
+    <t>Raising Hell</t>
+  </si>
+  <si>
+    <t>Tougher Than Leather</t>
+  </si>
+  <si>
+    <t>Back from Hell</t>
+  </si>
+  <si>
+    <t>Down with the King</t>
+  </si>
+  <si>
+    <t>Boogie Down Productions</t>
+  </si>
+  <si>
+    <t>Criminal Minded</t>
+  </si>
+  <si>
+    <t>By All Means Necessary</t>
+  </si>
+  <si>
+    <t>Ghetto Music: The Blueprint of Hip Hop</t>
+  </si>
+  <si>
+    <t>Edutainment</t>
+  </si>
+  <si>
+    <t>Sex and Violence</t>
+  </si>
+  <si>
+    <t>The Bronx</t>
+  </si>
+  <si>
+    <t>KRS-One</t>
+  </si>
+  <si>
+    <t>I M A M C R U 1 2</t>
+  </si>
+  <si>
+    <t>Return of the Boom Bap</t>
+  </si>
+  <si>
+    <t>I Got Next</t>
+  </si>
+  <si>
+    <t>The Sneak Attack</t>
+  </si>
+  <si>
+    <t>Spiritual Minded</t>
+  </si>
+  <si>
+    <t>Kristyles</t>
+  </si>
+  <si>
+    <t>Keep Right</t>
+  </si>
+  <si>
+    <t>Life</t>
+  </si>
+  <si>
+    <t>Adventures in Emceein</t>
+  </si>
+  <si>
+    <t>Maximum Strength</t>
+  </si>
+  <si>
+    <t>The BDP Album</t>
+  </si>
+  <si>
+    <t>Never Forget</t>
+  </si>
+  <si>
+    <t>Now Hear This</t>
+  </si>
+  <si>
+    <t>The World Is Mind</t>
+  </si>
+  <si>
+    <t>Street Light (First Edition)</t>
+  </si>
+  <si>
+    <t>Between Da Protests</t>
+  </si>
+  <si>
+    <t>Fat Joe</t>
+  </si>
+  <si>
+    <t>Represent</t>
+  </si>
+  <si>
+    <t>Jealous One's Envy</t>
+  </si>
+  <si>
+    <t>Don Cartagena</t>
+  </si>
+  <si>
+    <t>Jealous Ones Still Envy (J.O.S.E.)</t>
+  </si>
+  <si>
+    <t>Loyalty</t>
+  </si>
+  <si>
+    <t>All or Nothing</t>
+  </si>
+  <si>
+    <t>Me, Myself &amp; I</t>
+  </si>
+  <si>
+    <t>The Elephant in the Room</t>
+  </si>
+  <si>
+    <t>Jealous Ones Still Envy 2 (J.O.S.E. 2)</t>
+  </si>
+  <si>
+    <t>The Darkside Vol. 1</t>
+  </si>
+  <si>
+    <t>Queen Latifah</t>
+  </si>
+  <si>
+    <t>Persona</t>
+  </si>
+  <si>
+    <t>All Hail the Queen</t>
+  </si>
+  <si>
+    <t>Nature of a Sista'</t>
+  </si>
+  <si>
+    <t>Black Reign</t>
+  </si>
+  <si>
+    <t>Order in the Court</t>
+  </si>
+  <si>
+    <t>The Dana Owens Album</t>
+  </si>
+  <si>
+    <t>Trav'lin' Light</t>
+  </si>
+  <si>
+    <t>Joey Badass</t>
+  </si>
+  <si>
+    <t>B4.Da.$$</t>
+  </si>
+  <si>
+    <t>All-Amerikkkan Badass</t>
+  </si>
+  <si>
+    <t>Summer Knights</t>
+  </si>
+  <si>
+    <t>The Notorious B.I.G</t>
+  </si>
+  <si>
+    <t>Life After Death</t>
+  </si>
+  <si>
+    <t>Ready to Die</t>
+  </si>
+  <si>
+    <t>Born Again</t>
+  </si>
+  <si>
+    <t>Cam'ron</t>
+  </si>
+  <si>
+    <t>Purple Haze 2</t>
+  </si>
+  <si>
+    <t>Confessions of Fire</t>
+  </si>
+  <si>
+    <t>S.D.E.</t>
+  </si>
+  <si>
+    <t>Come Home with Me</t>
+  </si>
+  <si>
+    <t>Purple Haze</t>
+  </si>
+  <si>
+    <t>Killa Season</t>
+  </si>
+  <si>
+    <t>Crime Pays</t>
+  </si>
+  <si>
+    <t>Manhattan</t>
+  </si>
+  <si>
+    <t>Mobb Deep</t>
+  </si>
+  <si>
+    <t>The Infamous Mobb Deep</t>
+  </si>
+  <si>
+    <t>Juvenile Hell</t>
+  </si>
+  <si>
+    <t>The Infamous</t>
+  </si>
+  <si>
+    <t>Hell on Earth</t>
+  </si>
+  <si>
+    <t>Murda Muzik</t>
+  </si>
+  <si>
+    <t>Infamy</t>
+  </si>
+  <si>
+    <t>Amerikaz Nightmare</t>
+  </si>
+  <si>
+    <t>Blood Money</t>
+  </si>
+  <si>
+    <t>Lil' Kim</t>
+  </si>
+  <si>
+    <t>Hard Core</t>
+  </si>
+  <si>
+    <t>The Notorious K.I.M.</t>
+  </si>
+  <si>
+    <t>La Bella Mafia</t>
+  </si>
+  <si>
+    <t>The Naked Truth</t>
+  </si>
+  <si>
+    <t>Cardi B</t>
+  </si>
+  <si>
+    <t>Gangsta Bitch Music, Vol. 1</t>
+  </si>
+  <si>
+    <t>Gangsta Bitch Music, Vol. 2</t>
+  </si>
+  <si>
+    <t>Invasion of Privacy</t>
+  </si>
+  <si>
+    <t>Nicki Minaj</t>
+  </si>
+  <si>
+    <t>Pink Friday 2</t>
+  </si>
+  <si>
+    <t>Pink Friday</t>
+  </si>
+  <si>
+    <t>Pink Friday: Roman Reloaded</t>
+  </si>
+  <si>
+    <t>The Pinkprint</t>
+  </si>
+  <si>
+    <t>Queen</t>
+  </si>
+  <si>
+    <t>Beam Me Up Scotty</t>
+  </si>
+  <si>
+    <t>Beastie Boys</t>
+  </si>
+  <si>
+    <t>Hot Sauce Committee Part Two</t>
+  </si>
+  <si>
+    <t>Licensed to Ill</t>
+  </si>
+  <si>
+    <t>Paul's Boutique</t>
+  </si>
+  <si>
+    <t>Check Your Head</t>
+  </si>
+  <si>
+    <t>Ill Communication</t>
+  </si>
+  <si>
+    <t>Hello Nasty</t>
+  </si>
+  <si>
+    <t>To the 5 Boroughs</t>
+  </si>
+  <si>
+    <t>The Mix-Up</t>
+  </si>
+  <si>
+    <t>Remy Ma</t>
+  </si>
+  <si>
+    <t>There's Something About Remy: Based on a True Story</t>
+  </si>
+  <si>
+    <t>Animal Ambition</t>
+  </si>
+  <si>
+    <t>Get Rich or Die Tryin'</t>
+  </si>
+  <si>
+    <t>The Massacre</t>
+  </si>
+  <si>
+    <t>Curtis</t>
+  </si>
+  <si>
+    <t>Before I Self Destruct</t>
+  </si>
+  <si>
+    <t>50 Cent</t>
+  </si>
+  <si>
+    <t>Extinction Level Event 2: The Wrath of God</t>
+  </si>
+  <si>
+    <t>Busta Rhymes</t>
+  </si>
+  <si>
+    <t>The Coming</t>
+  </si>
+  <si>
+    <t>When Disaster Strikes…</t>
+  </si>
+  <si>
+    <t>Extinction Level Event: The Final World Front</t>
+  </si>
+  <si>
+    <t>Anarchy</t>
+  </si>
+  <si>
+    <t>Genesis</t>
+  </si>
+  <si>
+    <t>It Ain't Safe No More…</t>
+  </si>
+  <si>
+    <t>The Big Bang</t>
+  </si>
+  <si>
+    <t>Back on My B.S.</t>
+  </si>
+  <si>
+    <t>Year of the Dragon</t>
+  </si>
+  <si>
+    <t>Grandmaster Flash and the Furious Five</t>
+  </si>
+  <si>
+    <t>On the Strength</t>
+  </si>
+  <si>
+    <t>The Message</t>
+  </si>
+  <si>
+    <t>DMX</t>
+  </si>
+  <si>
+    <t>Exodus</t>
+  </si>
+  <si>
+    <t>Yonkers</t>
+  </si>
+  <si>
+    <t>It's Dark and Hell Is Hot</t>
+  </si>
+  <si>
+    <t>Flesh of My Flesh, Blood of My Blood</t>
+  </si>
+  <si>
+    <t>... And Then There Was X</t>
+  </si>
+  <si>
+    <t>The Great Depression</t>
+  </si>
+  <si>
+    <t>Grand Champ</t>
+  </si>
+  <si>
+    <t>Year of the Dog... Again</t>
+  </si>
+  <si>
+    <t>Undisputed</t>
+  </si>
+  <si>
+    <t>Young M.A</t>
+  </si>
+  <si>
+    <t>Herstory in the Making</t>
+  </si>
+  <si>
+    <t>Off the Yak</t>
+  </si>
+  <si>
+    <t>M.A The Mixtape</t>
+  </si>
+  <si>
+    <t>Sleep Walkin'</t>
+  </si>
+  <si>
+    <t>Don't Sweat the Technique</t>
+  </si>
+  <si>
+    <t>Eric B. &amp; Rakim</t>
+  </si>
+  <si>
+    <t>Paid in Full</t>
+  </si>
+  <si>
+    <t>Follow the Leader</t>
+  </si>
+  <si>
+    <t>Let the Rhythm Hit 'Em</t>
+  </si>
+  <si>
+    <t>Long Island</t>
+  </si>
+  <si>
+    <t>De La Soul</t>
+  </si>
+  <si>
+    <t>3 Feet High and Rising</t>
+  </si>
+  <si>
+    <t>De La Soul Is Dead</t>
+  </si>
+  <si>
+    <t>Buhloone Mindstate</t>
+  </si>
+  <si>
+    <t>Stakes Is High</t>
+  </si>
+  <si>
+    <t>Art Official Intelligence: Mosaic Thump</t>
+  </si>
+  <si>
+    <t>AOI: Bionix</t>
+  </si>
+  <si>
+    <t>The Grind Date</t>
+  </si>
+  <si>
+    <t>Plug 1 &amp; Plug 2 Present... First Serve</t>
+  </si>
+  <si>
+    <t>And the Anonymous Nobody…</t>
+  </si>
+  <si>
+    <t>Public Enemy</t>
+  </si>
+  <si>
+    <t>Nothing Is Quick in the Desert</t>
+  </si>
+  <si>
+    <t>Yo! Bum Rush the Show</t>
+  </si>
+  <si>
+    <t>It Takes a Nation of Millions to Hold Us Back</t>
+  </si>
+  <si>
+    <t>Fear of a Black Planet</t>
+  </si>
+  <si>
+    <t>Apocalypse 91... The Enemy Strikes Black</t>
+  </si>
+  <si>
+    <t>Muse Sick-n-Hour Mess Age</t>
+  </si>
+  <si>
+    <t>There's a Poison Goin' On</t>
+  </si>
+  <si>
+    <t>Revolverlution</t>
+  </si>
+  <si>
+    <t>New Whirl Odor</t>
+  </si>
+  <si>
+    <t>How You Sell Soul to a Soulless People Who Sold Their Soul?</t>
+  </si>
+  <si>
+    <t>Most of My Heroes Still Don't Appear on No Stamp</t>
+  </si>
+  <si>
+    <t>The Evil Empire of Everything</t>
+  </si>
+  <si>
+    <t>Man Plans God Laughs</t>
+  </si>
+  <si>
+    <t>Big Daddy Kane</t>
+  </si>
+  <si>
+    <t>Veteranz' Day</t>
+  </si>
+  <si>
+    <t>Long Live the Kane</t>
+  </si>
+  <si>
+    <t>It's a Big Daddy Thing</t>
+  </si>
+  <si>
+    <t>Taste of Chocolate</t>
+  </si>
+  <si>
+    <t>Prince of Darkness</t>
+  </si>
+  <si>
+    <t>Looks Like a Job For…</t>
+  </si>
+  <si>
+    <t>Daddy's Home</t>
+  </si>
+  <si>
+    <t>MF Doom</t>
+  </si>
+  <si>
+    <t>Born Like This</t>
+  </si>
+  <si>
+    <t>Operation: Doomsday</t>
+  </si>
+  <si>
+    <t>King Geedorah</t>
+  </si>
+  <si>
+    <t>Take Me to Your Leader</t>
+  </si>
+  <si>
+    <t>Vaudeville Villain</t>
+  </si>
+  <si>
+    <t>Viktor Vaughn</t>
+  </si>
+  <si>
+    <t>VV:2</t>
+  </si>
+  <si>
+    <t>Mm..Food</t>
+  </si>
+  <si>
+    <t>Kurtis Blow</t>
+  </si>
+  <si>
+    <t>Deuce</t>
+  </si>
+  <si>
+    <t>Tough</t>
+  </si>
+  <si>
+    <t>The Best Rapper on the Scene</t>
+  </si>
+  <si>
+    <t>Ego Trip</t>
+  </si>
+  <si>
+    <t>America</t>
+  </si>
+  <si>
+    <t>Kingdom Blow</t>
+  </si>
+  <si>
+    <t>Back by Popular Demand</t>
+  </si>
+  <si>
+    <t>Kanye West</t>
+  </si>
+  <si>
+    <t>Lupe Fiasco</t>
+  </si>
+  <si>
+    <t>Common</t>
+  </si>
+  <si>
+    <t>Kid Cudi</t>
+  </si>
+  <si>
+    <t>Eminem</t>
+  </si>
+  <si>
+    <t>Atmosphere</t>
+  </si>
+  <si>
+    <t>Brother Ali</t>
+  </si>
+  <si>
+    <t>Nelly</t>
+  </si>
+  <si>
+    <t>Tech N9ne</t>
+  </si>
+  <si>
+    <t>Chance the Rapper</t>
+  </si>
+  <si>
+    <t>Chief Keef</t>
   </si>
 </sst>
 </file>
@@ -1697,10 +2390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71A19CDE-E3DD-497E-8468-EF613F78BA90}">
-  <dimension ref="A1:E342"/>
+  <dimension ref="A1:E544"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A229" workbookViewId="0">
-      <selection activeCell="H243" sqref="H243"/>
+    <sheetView tabSelected="1" topLeftCell="A520" workbookViewId="0">
+      <selection activeCell="E534" sqref="E534"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7515,6 +8208,3308 @@
         <v>268</v>
       </c>
     </row>
+    <row r="343" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A343" t="s">
+        <v>423</v>
+      </c>
+      <c r="B343" t="s">
+        <v>425</v>
+      </c>
+      <c r="C343" t="s">
+        <v>278</v>
+      </c>
+      <c r="D343" t="s">
+        <v>279</v>
+      </c>
+      <c r="E343" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="344" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A344" t="s">
+        <v>423</v>
+      </c>
+      <c r="B344" t="s">
+        <v>424</v>
+      </c>
+      <c r="C344" t="s">
+        <v>278</v>
+      </c>
+      <c r="D344" t="s">
+        <v>279</v>
+      </c>
+      <c r="E344" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="345" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A345" t="s">
+        <v>426</v>
+      </c>
+      <c r="B345" t="s">
+        <v>428</v>
+      </c>
+      <c r="C345" t="s">
+        <v>274</v>
+      </c>
+      <c r="D345" t="s">
+        <v>275</v>
+      </c>
+      <c r="E345" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="346" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A346" t="s">
+        <v>426</v>
+      </c>
+      <c r="B346" t="s">
+        <v>427</v>
+      </c>
+      <c r="C346" t="s">
+        <v>274</v>
+      </c>
+      <c r="D346" t="s">
+        <v>275</v>
+      </c>
+      <c r="E346" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="347" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A347" t="s">
+        <v>429</v>
+      </c>
+      <c r="B347" t="s">
+        <v>431</v>
+      </c>
+      <c r="C347" t="s">
+        <v>422</v>
+      </c>
+      <c r="D347" t="s">
+        <v>340</v>
+      </c>
+      <c r="E347" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="348" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A348" t="s">
+        <v>429</v>
+      </c>
+      <c r="B348" t="s">
+        <v>432</v>
+      </c>
+      <c r="C348" t="s">
+        <v>422</v>
+      </c>
+      <c r="D348" t="s">
+        <v>340</v>
+      </c>
+      <c r="E348" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="349" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A349" t="s">
+        <v>429</v>
+      </c>
+      <c r="B349" t="s">
+        <v>435</v>
+      </c>
+      <c r="C349" t="s">
+        <v>422</v>
+      </c>
+      <c r="D349" t="s">
+        <v>340</v>
+      </c>
+      <c r="E349" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="350" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A350" t="s">
+        <v>429</v>
+      </c>
+      <c r="B350" t="s">
+        <v>433</v>
+      </c>
+      <c r="C350" t="s">
+        <v>422</v>
+      </c>
+      <c r="D350" t="s">
+        <v>340</v>
+      </c>
+      <c r="E350" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="351" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A351" t="s">
+        <v>429</v>
+      </c>
+      <c r="B351" t="s">
+        <v>434</v>
+      </c>
+      <c r="C351" t="s">
+        <v>422</v>
+      </c>
+      <c r="D351" t="s">
+        <v>340</v>
+      </c>
+      <c r="E351" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="352" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A352" t="s">
+        <v>429</v>
+      </c>
+      <c r="B352" t="s">
+        <v>430</v>
+      </c>
+      <c r="C352" t="s">
+        <v>422</v>
+      </c>
+      <c r="D352" t="s">
+        <v>340</v>
+      </c>
+      <c r="E352" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="353" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A353" t="s">
+        <v>436</v>
+      </c>
+      <c r="B353" t="s">
+        <v>438</v>
+      </c>
+      <c r="C353" t="s">
+        <v>422</v>
+      </c>
+      <c r="D353" t="s">
+        <v>340</v>
+      </c>
+      <c r="E353" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="354" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A354" t="s">
+        <v>436</v>
+      </c>
+      <c r="B354" t="s">
+        <v>439</v>
+      </c>
+      <c r="C354" t="s">
+        <v>422</v>
+      </c>
+      <c r="D354" t="s">
+        <v>340</v>
+      </c>
+      <c r="E354" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="355" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A355" t="s">
+        <v>436</v>
+      </c>
+      <c r="B355" t="s">
+        <v>440</v>
+      </c>
+      <c r="C355" t="s">
+        <v>422</v>
+      </c>
+      <c r="D355" t="s">
+        <v>340</v>
+      </c>
+      <c r="E355" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="356" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A356" t="s">
+        <v>436</v>
+      </c>
+      <c r="B356" t="s">
+        <v>441</v>
+      </c>
+      <c r="C356" t="s">
+        <v>422</v>
+      </c>
+      <c r="D356" t="s">
+        <v>340</v>
+      </c>
+      <c r="E356" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="357" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A357" t="s">
+        <v>436</v>
+      </c>
+      <c r="B357" t="s">
+        <v>442</v>
+      </c>
+      <c r="C357" t="s">
+        <v>422</v>
+      </c>
+      <c r="D357" t="s">
+        <v>340</v>
+      </c>
+      <c r="E357" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="358" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A358" t="s">
+        <v>436</v>
+      </c>
+      <c r="B358" t="s">
+        <v>443</v>
+      </c>
+      <c r="C358" t="s">
+        <v>422</v>
+      </c>
+      <c r="D358" t="s">
+        <v>340</v>
+      </c>
+      <c r="E358" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="359" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A359" t="s">
+        <v>436</v>
+      </c>
+      <c r="B359" t="s">
+        <v>444</v>
+      </c>
+      <c r="C359" t="s">
+        <v>422</v>
+      </c>
+      <c r="D359" t="s">
+        <v>340</v>
+      </c>
+      <c r="E359" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="360" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A360" t="s">
+        <v>436</v>
+      </c>
+      <c r="B360" t="s">
+        <v>445</v>
+      </c>
+      <c r="C360" t="s">
+        <v>422</v>
+      </c>
+      <c r="D360" t="s">
+        <v>340</v>
+      </c>
+      <c r="E360" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="361" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A361" t="s">
+        <v>436</v>
+      </c>
+      <c r="B361" s="3">
+        <v>10</v>
+      </c>
+      <c r="C361" t="s">
+        <v>422</v>
+      </c>
+      <c r="D361" t="s">
+        <v>340</v>
+      </c>
+      <c r="E361" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="362" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A362" t="s">
+        <v>436</v>
+      </c>
+      <c r="B362" t="s">
+        <v>446</v>
+      </c>
+      <c r="C362" t="s">
+        <v>422</v>
+      </c>
+      <c r="D362" t="s">
+        <v>340</v>
+      </c>
+      <c r="E362" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="363" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A363" t="s">
+        <v>436</v>
+      </c>
+      <c r="B363" t="s">
+        <v>447</v>
+      </c>
+      <c r="C363" t="s">
+        <v>422</v>
+      </c>
+      <c r="D363" t="s">
+        <v>340</v>
+      </c>
+      <c r="E363" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="364" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A364" t="s">
+        <v>436</v>
+      </c>
+      <c r="B364" t="s">
+        <v>448</v>
+      </c>
+      <c r="C364" t="s">
+        <v>422</v>
+      </c>
+      <c r="D364" t="s">
+        <v>340</v>
+      </c>
+      <c r="E364" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="365" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A365" t="s">
+        <v>436</v>
+      </c>
+      <c r="B365" t="s">
+        <v>437</v>
+      </c>
+      <c r="C365" t="s">
+        <v>422</v>
+      </c>
+      <c r="D365" t="s">
+        <v>340</v>
+      </c>
+      <c r="E365" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="366" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A366" t="s">
+        <v>449</v>
+      </c>
+      <c r="B366" t="s">
+        <v>451</v>
+      </c>
+      <c r="C366" t="s">
+        <v>422</v>
+      </c>
+      <c r="D366" t="s">
+        <v>340</v>
+      </c>
+      <c r="E366" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="367" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A367" t="s">
+        <v>449</v>
+      </c>
+      <c r="B367" t="s">
+        <v>452</v>
+      </c>
+      <c r="C367" t="s">
+        <v>422</v>
+      </c>
+      <c r="D367" t="s">
+        <v>340</v>
+      </c>
+      <c r="E367" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="368" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A368" t="s">
+        <v>449</v>
+      </c>
+      <c r="B368" t="s">
+        <v>453</v>
+      </c>
+      <c r="C368" t="s">
+        <v>422</v>
+      </c>
+      <c r="D368" t="s">
+        <v>340</v>
+      </c>
+      <c r="E368" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="369" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A369" t="s">
+        <v>449</v>
+      </c>
+      <c r="B369" t="s">
+        <v>454</v>
+      </c>
+      <c r="C369" t="s">
+        <v>422</v>
+      </c>
+      <c r="D369" t="s">
+        <v>340</v>
+      </c>
+      <c r="E369" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="370" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A370" t="s">
+        <v>449</v>
+      </c>
+      <c r="B370" t="s">
+        <v>455</v>
+      </c>
+      <c r="C370" t="s">
+        <v>422</v>
+      </c>
+      <c r="D370" t="s">
+        <v>340</v>
+      </c>
+      <c r="E370" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="371" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A371" t="s">
+        <v>449</v>
+      </c>
+      <c r="B371" t="s">
+        <v>456</v>
+      </c>
+      <c r="C371" t="s">
+        <v>422</v>
+      </c>
+      <c r="D371" t="s">
+        <v>340</v>
+      </c>
+      <c r="E371" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="372" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A372" t="s">
+        <v>449</v>
+      </c>
+      <c r="B372" t="s">
+        <v>450</v>
+      </c>
+      <c r="C372" t="s">
+        <v>422</v>
+      </c>
+      <c r="D372" t="s">
+        <v>340</v>
+      </c>
+      <c r="E372" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="373" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A373" t="s">
+        <v>457</v>
+      </c>
+      <c r="B373" t="s">
+        <v>458</v>
+      </c>
+      <c r="C373" t="s">
+        <v>463</v>
+      </c>
+      <c r="D373" t="s">
+        <v>340</v>
+      </c>
+      <c r="E373" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="374" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A374" t="s">
+        <v>457</v>
+      </c>
+      <c r="B374" t="s">
+        <v>459</v>
+      </c>
+      <c r="C374" t="s">
+        <v>463</v>
+      </c>
+      <c r="D374" t="s">
+        <v>340</v>
+      </c>
+      <c r="E374" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="375" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A375" t="s">
+        <v>457</v>
+      </c>
+      <c r="B375" t="s">
+        <v>460</v>
+      </c>
+      <c r="C375" t="s">
+        <v>463</v>
+      </c>
+      <c r="D375" t="s">
+        <v>340</v>
+      </c>
+      <c r="E375" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="376" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A376" t="s">
+        <v>457</v>
+      </c>
+      <c r="B376" t="s">
+        <v>461</v>
+      </c>
+      <c r="C376" t="s">
+        <v>463</v>
+      </c>
+      <c r="D376" t="s">
+        <v>340</v>
+      </c>
+      <c r="E376" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="377" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A377" t="s">
+        <v>457</v>
+      </c>
+      <c r="B377" t="s">
+        <v>462</v>
+      </c>
+      <c r="C377" t="s">
+        <v>463</v>
+      </c>
+      <c r="D377" t="s">
+        <v>340</v>
+      </c>
+      <c r="E377" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="378" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A378" t="s">
+        <v>464</v>
+      </c>
+      <c r="B378" t="s">
+        <v>466</v>
+      </c>
+      <c r="C378" t="s">
+        <v>463</v>
+      </c>
+      <c r="D378" t="s">
+        <v>340</v>
+      </c>
+      <c r="E378" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="379" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A379" t="s">
+        <v>464</v>
+      </c>
+      <c r="B379" t="s">
+        <v>464</v>
+      </c>
+      <c r="C379" t="s">
+        <v>463</v>
+      </c>
+      <c r="D379" t="s">
+        <v>340</v>
+      </c>
+      <c r="E379" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="380" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A380" t="s">
+        <v>464</v>
+      </c>
+      <c r="B380" t="s">
+        <v>467</v>
+      </c>
+      <c r="C380" t="s">
+        <v>463</v>
+      </c>
+      <c r="D380" t="s">
+        <v>340</v>
+      </c>
+      <c r="E380" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="381" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A381" t="s">
+        <v>464</v>
+      </c>
+      <c r="B381" t="s">
+        <v>468</v>
+      </c>
+      <c r="C381" t="s">
+        <v>463</v>
+      </c>
+      <c r="D381" t="s">
+        <v>340</v>
+      </c>
+      <c r="E381" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="382" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A382" t="s">
+        <v>464</v>
+      </c>
+      <c r="B382" t="s">
+        <v>469</v>
+      </c>
+      <c r="C382" t="s">
+        <v>463</v>
+      </c>
+      <c r="D382" t="s">
+        <v>340</v>
+      </c>
+      <c r="E382" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="383" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A383" t="s">
+        <v>464</v>
+      </c>
+      <c r="B383" t="s">
+        <v>470</v>
+      </c>
+      <c r="C383" t="s">
+        <v>463</v>
+      </c>
+      <c r="D383" t="s">
+        <v>340</v>
+      </c>
+      <c r="E383" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="384" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A384" t="s">
+        <v>464</v>
+      </c>
+      <c r="B384" t="s">
+        <v>471</v>
+      </c>
+      <c r="C384" t="s">
+        <v>463</v>
+      </c>
+      <c r="D384" t="s">
+        <v>340</v>
+      </c>
+      <c r="E384" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="385" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A385" t="s">
+        <v>464</v>
+      </c>
+      <c r="B385" t="s">
+        <v>472</v>
+      </c>
+      <c r="C385" t="s">
+        <v>463</v>
+      </c>
+      <c r="D385" t="s">
+        <v>340</v>
+      </c>
+      <c r="E385" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="386" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A386" t="s">
+        <v>464</v>
+      </c>
+      <c r="B386" t="s">
+        <v>473</v>
+      </c>
+      <c r="C386" t="s">
+        <v>463</v>
+      </c>
+      <c r="D386" t="s">
+        <v>340</v>
+      </c>
+      <c r="E386" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="387" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A387" t="s">
+        <v>464</v>
+      </c>
+      <c r="B387" t="s">
+        <v>474</v>
+      </c>
+      <c r="C387" t="s">
+        <v>463</v>
+      </c>
+      <c r="D387" t="s">
+        <v>340</v>
+      </c>
+      <c r="E387" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="388" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A388" t="s">
+        <v>464</v>
+      </c>
+      <c r="B388" t="s">
+        <v>475</v>
+      </c>
+      <c r="C388" t="s">
+        <v>463</v>
+      </c>
+      <c r="D388" t="s">
+        <v>340</v>
+      </c>
+      <c r="E388" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="389" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A389" t="s">
+        <v>464</v>
+      </c>
+      <c r="B389" t="s">
+        <v>476</v>
+      </c>
+      <c r="C389" t="s">
+        <v>463</v>
+      </c>
+      <c r="D389" t="s">
+        <v>340</v>
+      </c>
+      <c r="E389" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="390" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A390" t="s">
+        <v>464</v>
+      </c>
+      <c r="B390" t="s">
+        <v>477</v>
+      </c>
+      <c r="C390" t="s">
+        <v>463</v>
+      </c>
+      <c r="D390" t="s">
+        <v>340</v>
+      </c>
+      <c r="E390" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="391" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A391" t="s">
+        <v>464</v>
+      </c>
+      <c r="B391" t="s">
+        <v>478</v>
+      </c>
+      <c r="C391" t="s">
+        <v>463</v>
+      </c>
+      <c r="D391" t="s">
+        <v>340</v>
+      </c>
+      <c r="E391" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="392" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A392" t="s">
+        <v>464</v>
+      </c>
+      <c r="B392" t="s">
+        <v>479</v>
+      </c>
+      <c r="C392" t="s">
+        <v>463</v>
+      </c>
+      <c r="D392" t="s">
+        <v>340</v>
+      </c>
+      <c r="E392" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="393" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A393" t="s">
+        <v>464</v>
+      </c>
+      <c r="B393" t="s">
+        <v>480</v>
+      </c>
+      <c r="C393" t="s">
+        <v>463</v>
+      </c>
+      <c r="D393" t="s">
+        <v>340</v>
+      </c>
+      <c r="E393" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="394" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A394" t="s">
+        <v>464</v>
+      </c>
+      <c r="B394" t="s">
+        <v>465</v>
+      </c>
+      <c r="C394" t="s">
+        <v>463</v>
+      </c>
+      <c r="D394" t="s">
+        <v>340</v>
+      </c>
+      <c r="E394" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="395" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A395" t="s">
+        <v>481</v>
+      </c>
+      <c r="B395" t="s">
+        <v>482</v>
+      </c>
+      <c r="C395" t="s">
+        <v>463</v>
+      </c>
+      <c r="D395" t="s">
+        <v>340</v>
+      </c>
+      <c r="E395" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="396" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A396" t="s">
+        <v>481</v>
+      </c>
+      <c r="B396" t="s">
+        <v>483</v>
+      </c>
+      <c r="C396" t="s">
+        <v>463</v>
+      </c>
+      <c r="D396" t="s">
+        <v>340</v>
+      </c>
+      <c r="E396" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="397" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A397" t="s">
+        <v>481</v>
+      </c>
+      <c r="B397" t="s">
+        <v>484</v>
+      </c>
+      <c r="C397" t="s">
+        <v>463</v>
+      </c>
+      <c r="D397" t="s">
+        <v>340</v>
+      </c>
+      <c r="E397" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="398" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A398" t="s">
+        <v>481</v>
+      </c>
+      <c r="B398" t="s">
+        <v>485</v>
+      </c>
+      <c r="C398" t="s">
+        <v>463</v>
+      </c>
+      <c r="D398" t="s">
+        <v>340</v>
+      </c>
+      <c r="E398" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="399" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A399" t="s">
+        <v>481</v>
+      </c>
+      <c r="B399" t="s">
+        <v>486</v>
+      </c>
+      <c r="C399" t="s">
+        <v>463</v>
+      </c>
+      <c r="D399" t="s">
+        <v>340</v>
+      </c>
+      <c r="E399" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="400" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A400" t="s">
+        <v>481</v>
+      </c>
+      <c r="B400" t="s">
+        <v>487</v>
+      </c>
+      <c r="C400" t="s">
+        <v>463</v>
+      </c>
+      <c r="D400" t="s">
+        <v>340</v>
+      </c>
+      <c r="E400" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="401" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A401" t="s">
+        <v>481</v>
+      </c>
+      <c r="B401" t="s">
+        <v>488</v>
+      </c>
+      <c r="C401" t="s">
+        <v>463</v>
+      </c>
+      <c r="D401" t="s">
+        <v>340</v>
+      </c>
+      <c r="E401" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="402" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A402" t="s">
+        <v>481</v>
+      </c>
+      <c r="B402" t="s">
+        <v>489</v>
+      </c>
+      <c r="C402" t="s">
+        <v>463</v>
+      </c>
+      <c r="D402" t="s">
+        <v>340</v>
+      </c>
+      <c r="E402" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="403" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A403" t="s">
+        <v>481</v>
+      </c>
+      <c r="B403" t="s">
+        <v>490</v>
+      </c>
+      <c r="C403" t="s">
+        <v>463</v>
+      </c>
+      <c r="D403" t="s">
+        <v>340</v>
+      </c>
+      <c r="E403" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="404" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A404" t="s">
+        <v>481</v>
+      </c>
+      <c r="B404" t="s">
+        <v>491</v>
+      </c>
+      <c r="C404" t="s">
+        <v>463</v>
+      </c>
+      <c r="D404" t="s">
+        <v>340</v>
+      </c>
+      <c r="E404" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="405" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A405" t="s">
+        <v>492</v>
+      </c>
+      <c r="B405" t="s">
+        <v>494</v>
+      </c>
+      <c r="C405" t="s">
+        <v>361</v>
+      </c>
+      <c r="D405" t="s">
+        <v>362</v>
+      </c>
+      <c r="E405" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="406" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A406" t="s">
+        <v>492</v>
+      </c>
+      <c r="B406" t="s">
+        <v>495</v>
+      </c>
+      <c r="C406" t="s">
+        <v>361</v>
+      </c>
+      <c r="D406" t="s">
+        <v>362</v>
+      </c>
+      <c r="E406" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="407" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A407" t="s">
+        <v>492</v>
+      </c>
+      <c r="B407" t="s">
+        <v>496</v>
+      </c>
+      <c r="C407" t="s">
+        <v>361</v>
+      </c>
+      <c r="D407" t="s">
+        <v>362</v>
+      </c>
+      <c r="E407" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="408" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A408" t="s">
+        <v>492</v>
+      </c>
+      <c r="B408" t="s">
+        <v>497</v>
+      </c>
+      <c r="C408" t="s">
+        <v>361</v>
+      </c>
+      <c r="D408" t="s">
+        <v>362</v>
+      </c>
+      <c r="E408" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="409" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A409" t="s">
+        <v>492</v>
+      </c>
+      <c r="B409" t="s">
+        <v>498</v>
+      </c>
+      <c r="C409" t="s">
+        <v>361</v>
+      </c>
+      <c r="D409" t="s">
+        <v>362</v>
+      </c>
+      <c r="E409" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="410" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A410" t="s">
+        <v>492</v>
+      </c>
+      <c r="B410" t="s">
+        <v>499</v>
+      </c>
+      <c r="C410" t="s">
+        <v>361</v>
+      </c>
+      <c r="D410" t="s">
+        <v>362</v>
+      </c>
+      <c r="E410" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="411" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A411" t="s">
+        <v>492</v>
+      </c>
+      <c r="B411" t="s">
+        <v>493</v>
+      </c>
+      <c r="C411" t="s">
+        <v>361</v>
+      </c>
+      <c r="D411" t="s">
+        <v>362</v>
+      </c>
+      <c r="E411" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="412" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A412" t="s">
+        <v>500</v>
+      </c>
+      <c r="B412" s="3" t="s">
+        <v>501</v>
+      </c>
+      <c r="C412" t="s">
+        <v>350</v>
+      </c>
+      <c r="D412" t="s">
+        <v>340</v>
+      </c>
+      <c r="E412" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="413" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A413" t="s">
+        <v>500</v>
+      </c>
+      <c r="B413" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="C413" t="s">
+        <v>350</v>
+      </c>
+      <c r="D413" t="s">
+        <v>340</v>
+      </c>
+      <c r="E413" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="414" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A414" t="s">
+        <v>500</v>
+      </c>
+      <c r="B414" s="3">
+        <v>2000</v>
+      </c>
+      <c r="C414" t="s">
+        <v>350</v>
+      </c>
+      <c r="D414" t="s">
+        <v>340</v>
+      </c>
+      <c r="E414" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="415" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A415" t="s">
+        <v>500</v>
+      </c>
+      <c r="B415" s="3">
+        <v>1999</v>
+      </c>
+      <c r="C415" t="s">
+        <v>350</v>
+      </c>
+      <c r="D415" t="s">
+        <v>340</v>
+      </c>
+      <c r="E415" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="416" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A416" t="s">
+        <v>500</v>
+      </c>
+      <c r="B416" s="3" t="s">
+        <v>503</v>
+      </c>
+      <c r="C416" t="s">
+        <v>350</v>
+      </c>
+      <c r="D416" t="s">
+        <v>340</v>
+      </c>
+      <c r="E416" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="417" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A417" t="s">
+        <v>504</v>
+      </c>
+      <c r="B417" t="s">
+        <v>506</v>
+      </c>
+      <c r="C417" t="s">
+        <v>350</v>
+      </c>
+      <c r="D417" t="s">
+        <v>340</v>
+      </c>
+      <c r="E417" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="418" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A418" t="s">
+        <v>504</v>
+      </c>
+      <c r="B418" t="s">
+        <v>505</v>
+      </c>
+      <c r="C418" t="s">
+        <v>350</v>
+      </c>
+      <c r="D418" t="s">
+        <v>340</v>
+      </c>
+      <c r="E418" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="419" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A419" t="s">
+        <v>504</v>
+      </c>
+      <c r="B419" s="3" t="s">
+        <v>507</v>
+      </c>
+      <c r="C419" t="s">
+        <v>350</v>
+      </c>
+      <c r="D419" t="s">
+        <v>340</v>
+      </c>
+      <c r="E419" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="420" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A420" t="s">
+        <v>508</v>
+      </c>
+      <c r="B420" t="s">
+        <v>510</v>
+      </c>
+      <c r="C420" t="s">
+        <v>516</v>
+      </c>
+      <c r="D420" t="s">
+        <v>340</v>
+      </c>
+      <c r="E420" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="421" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A421" t="s">
+        <v>508</v>
+      </c>
+      <c r="B421" t="s">
+        <v>511</v>
+      </c>
+      <c r="C421" t="s">
+        <v>516</v>
+      </c>
+      <c r="D421" t="s">
+        <v>340</v>
+      </c>
+      <c r="E421" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="422" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A422" t="s">
+        <v>508</v>
+      </c>
+      <c r="B422" t="s">
+        <v>512</v>
+      </c>
+      <c r="C422" t="s">
+        <v>516</v>
+      </c>
+      <c r="D422" t="s">
+        <v>340</v>
+      </c>
+      <c r="E422" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="423" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A423" t="s">
+        <v>508</v>
+      </c>
+      <c r="B423" t="s">
+        <v>513</v>
+      </c>
+      <c r="C423" t="s">
+        <v>516</v>
+      </c>
+      <c r="D423" t="s">
+        <v>340</v>
+      </c>
+      <c r="E423" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="424" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A424" t="s">
+        <v>508</v>
+      </c>
+      <c r="B424" t="s">
+        <v>514</v>
+      </c>
+      <c r="C424" t="s">
+        <v>516</v>
+      </c>
+      <c r="D424" t="s">
+        <v>340</v>
+      </c>
+      <c r="E424" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="425" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A425" t="s">
+        <v>508</v>
+      </c>
+      <c r="B425" t="s">
+        <v>515</v>
+      </c>
+      <c r="C425" t="s">
+        <v>516</v>
+      </c>
+      <c r="D425" t="s">
+        <v>340</v>
+      </c>
+      <c r="E425" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="426" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A426" t="s">
+        <v>508</v>
+      </c>
+      <c r="B426" t="s">
+        <v>509</v>
+      </c>
+      <c r="C426" t="s">
+        <v>516</v>
+      </c>
+      <c r="D426" t="s">
+        <v>340</v>
+      </c>
+      <c r="E426" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="427" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A427" t="s">
+        <v>517</v>
+      </c>
+      <c r="B427" t="s">
+        <v>519</v>
+      </c>
+      <c r="C427" t="s">
+        <v>422</v>
+      </c>
+      <c r="D427" t="s">
+        <v>340</v>
+      </c>
+      <c r="E427" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="428" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A428" t="s">
+        <v>517</v>
+      </c>
+      <c r="B428" t="s">
+        <v>520</v>
+      </c>
+      <c r="C428" t="s">
+        <v>422</v>
+      </c>
+      <c r="D428" t="s">
+        <v>340</v>
+      </c>
+      <c r="E428" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="429" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A429" t="s">
+        <v>517</v>
+      </c>
+      <c r="B429" t="s">
+        <v>521</v>
+      </c>
+      <c r="C429" t="s">
+        <v>422</v>
+      </c>
+      <c r="D429" t="s">
+        <v>340</v>
+      </c>
+      <c r="E429" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="430" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A430" t="s">
+        <v>517</v>
+      </c>
+      <c r="B430" t="s">
+        <v>522</v>
+      </c>
+      <c r="C430" t="s">
+        <v>422</v>
+      </c>
+      <c r="D430" t="s">
+        <v>340</v>
+      </c>
+      <c r="E430" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="431" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A431" t="s">
+        <v>517</v>
+      </c>
+      <c r="B431" t="s">
+        <v>523</v>
+      </c>
+      <c r="C431" t="s">
+        <v>422</v>
+      </c>
+      <c r="D431" t="s">
+        <v>340</v>
+      </c>
+      <c r="E431" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="432" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A432" t="s">
+        <v>517</v>
+      </c>
+      <c r="B432" t="s">
+        <v>524</v>
+      </c>
+      <c r="C432" t="s">
+        <v>422</v>
+      </c>
+      <c r="D432" t="s">
+        <v>340</v>
+      </c>
+      <c r="E432" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="433" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A433" t="s">
+        <v>517</v>
+      </c>
+      <c r="B433" t="s">
+        <v>525</v>
+      </c>
+      <c r="C433" t="s">
+        <v>422</v>
+      </c>
+      <c r="D433" t="s">
+        <v>340</v>
+      </c>
+      <c r="E433" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="434" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A434" t="s">
+        <v>517</v>
+      </c>
+      <c r="B434" t="s">
+        <v>518</v>
+      </c>
+      <c r="C434" t="s">
+        <v>422</v>
+      </c>
+      <c r="D434" t="s">
+        <v>340</v>
+      </c>
+      <c r="E434" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="435" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A435" t="s">
+        <v>526</v>
+      </c>
+      <c r="B435" s="3" t="s">
+        <v>527</v>
+      </c>
+      <c r="C435" t="s">
+        <v>350</v>
+      </c>
+      <c r="D435" t="s">
+        <v>340</v>
+      </c>
+      <c r="E435" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="436" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A436" t="s">
+        <v>526</v>
+      </c>
+      <c r="B436" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="C436" t="s">
+        <v>350</v>
+      </c>
+      <c r="D436" t="s">
+        <v>340</v>
+      </c>
+      <c r="E436" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="437" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A437" t="s">
+        <v>526</v>
+      </c>
+      <c r="B437" s="3" t="s">
+        <v>529</v>
+      </c>
+      <c r="C437" t="s">
+        <v>350</v>
+      </c>
+      <c r="D437" t="s">
+        <v>340</v>
+      </c>
+      <c r="E437" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="438" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A438" t="s">
+        <v>526</v>
+      </c>
+      <c r="B438" s="3" t="s">
+        <v>530</v>
+      </c>
+      <c r="C438" t="s">
+        <v>350</v>
+      </c>
+      <c r="D438" t="s">
+        <v>340</v>
+      </c>
+      <c r="E438" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="439" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A439" t="s">
+        <v>526</v>
+      </c>
+      <c r="B439" s="3">
+        <v>9</v>
+      </c>
+      <c r="C439" t="s">
+        <v>350</v>
+      </c>
+      <c r="D439" t="s">
+        <v>340</v>
+      </c>
+      <c r="E439" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="440" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A440" t="s">
+        <v>531</v>
+      </c>
+      <c r="B440" s="3" t="s">
+        <v>532</v>
+      </c>
+      <c r="C440" t="s">
+        <v>463</v>
+      </c>
+      <c r="D440" t="s">
+        <v>340</v>
+      </c>
+      <c r="E440" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="441" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A441" t="s">
+        <v>531</v>
+      </c>
+      <c r="B441" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="C441" t="s">
+        <v>463</v>
+      </c>
+      <c r="D441" t="s">
+        <v>340</v>
+      </c>
+      <c r="E441" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="442" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A442" t="s">
+        <v>531</v>
+      </c>
+      <c r="B442" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="C442" t="s">
+        <v>463</v>
+      </c>
+      <c r="D442" t="s">
+        <v>340</v>
+      </c>
+      <c r="E442" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="443" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A443" t="s">
+        <v>535</v>
+      </c>
+      <c r="B443" t="s">
+        <v>537</v>
+      </c>
+      <c r="C443" t="s">
+        <v>422</v>
+      </c>
+      <c r="D443" t="s">
+        <v>340</v>
+      </c>
+      <c r="E443" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="444" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A444" t="s">
+        <v>535</v>
+      </c>
+      <c r="B444" t="s">
+        <v>538</v>
+      </c>
+      <c r="C444" t="s">
+        <v>422</v>
+      </c>
+      <c r="D444" t="s">
+        <v>340</v>
+      </c>
+      <c r="E444" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="445" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A445" t="s">
+        <v>535</v>
+      </c>
+      <c r="B445" t="s">
+        <v>539</v>
+      </c>
+      <c r="C445" t="s">
+        <v>422</v>
+      </c>
+      <c r="D445" t="s">
+        <v>340</v>
+      </c>
+      <c r="E445" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="446" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A446" t="s">
+        <v>535</v>
+      </c>
+      <c r="B446" t="s">
+        <v>540</v>
+      </c>
+      <c r="C446" t="s">
+        <v>422</v>
+      </c>
+      <c r="D446" t="s">
+        <v>340</v>
+      </c>
+      <c r="E446" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="447" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A447" t="s">
+        <v>535</v>
+      </c>
+      <c r="B447" t="s">
+        <v>536</v>
+      </c>
+      <c r="C447" t="s">
+        <v>422</v>
+      </c>
+      <c r="D447" t="s">
+        <v>340</v>
+      </c>
+      <c r="E447" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="448" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A448" t="s">
+        <v>535</v>
+      </c>
+      <c r="B448" t="s">
+        <v>541</v>
+      </c>
+      <c r="C448" t="s">
+        <v>422</v>
+      </c>
+      <c r="D448" t="s">
+        <v>340</v>
+      </c>
+      <c r="E448" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="449" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A449" t="s">
+        <v>542</v>
+      </c>
+      <c r="B449" t="s">
+        <v>544</v>
+      </c>
+      <c r="C449" t="s">
+        <v>516</v>
+      </c>
+      <c r="D449" t="s">
+        <v>340</v>
+      </c>
+      <c r="E449" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="450" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A450" t="s">
+        <v>542</v>
+      </c>
+      <c r="B450" t="s">
+        <v>545</v>
+      </c>
+      <c r="C450" t="s">
+        <v>516</v>
+      </c>
+      <c r="D450" t="s">
+        <v>340</v>
+      </c>
+      <c r="E450" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="451" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A451" t="s">
+        <v>542</v>
+      </c>
+      <c r="B451" t="s">
+        <v>546</v>
+      </c>
+      <c r="C451" t="s">
+        <v>516</v>
+      </c>
+      <c r="D451" t="s">
+        <v>340</v>
+      </c>
+      <c r="E451" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="452" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A452" t="s">
+        <v>542</v>
+      </c>
+      <c r="B452" t="s">
+        <v>547</v>
+      </c>
+      <c r="C452" t="s">
+        <v>516</v>
+      </c>
+      <c r="D452" t="s">
+        <v>340</v>
+      </c>
+      <c r="E452" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="453" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A453" t="s">
+        <v>542</v>
+      </c>
+      <c r="B453" t="s">
+        <v>548</v>
+      </c>
+      <c r="C453" t="s">
+        <v>516</v>
+      </c>
+      <c r="D453" t="s">
+        <v>340</v>
+      </c>
+      <c r="E453" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="454" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A454" t="s">
+        <v>542</v>
+      </c>
+      <c r="B454" t="s">
+        <v>549</v>
+      </c>
+      <c r="C454" t="s">
+        <v>516</v>
+      </c>
+      <c r="D454" t="s">
+        <v>340</v>
+      </c>
+      <c r="E454" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="455" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A455" t="s">
+        <v>542</v>
+      </c>
+      <c r="B455" t="s">
+        <v>550</v>
+      </c>
+      <c r="C455" t="s">
+        <v>516</v>
+      </c>
+      <c r="D455" t="s">
+        <v>340</v>
+      </c>
+      <c r="E455" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="456" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A456" t="s">
+        <v>542</v>
+      </c>
+      <c r="B456" t="s">
+        <v>543</v>
+      </c>
+      <c r="C456" t="s">
+        <v>516</v>
+      </c>
+      <c r="D456" t="s">
+        <v>340</v>
+      </c>
+      <c r="E456" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="457" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A457" t="s">
+        <v>551</v>
+      </c>
+      <c r="B457" t="s">
+        <v>552</v>
+      </c>
+      <c r="C457" t="s">
+        <v>463</v>
+      </c>
+      <c r="D457" t="s">
+        <v>340</v>
+      </c>
+      <c r="E457" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="458" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A458" t="s">
+        <v>558</v>
+      </c>
+      <c r="B458" t="s">
+        <v>554</v>
+      </c>
+      <c r="C458" t="s">
+        <v>422</v>
+      </c>
+      <c r="D458" t="s">
+        <v>340</v>
+      </c>
+      <c r="E458" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="459" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A459" t="s">
+        <v>558</v>
+      </c>
+      <c r="B459" t="s">
+        <v>555</v>
+      </c>
+      <c r="C459" t="s">
+        <v>422</v>
+      </c>
+      <c r="D459" t="s">
+        <v>340</v>
+      </c>
+      <c r="E459" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="460" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A460" t="s">
+        <v>558</v>
+      </c>
+      <c r="B460" t="s">
+        <v>556</v>
+      </c>
+      <c r="C460" t="s">
+        <v>422</v>
+      </c>
+      <c r="D460" t="s">
+        <v>340</v>
+      </c>
+      <c r="E460" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="461" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A461" t="s">
+        <v>558</v>
+      </c>
+      <c r="B461" t="s">
+        <v>557</v>
+      </c>
+      <c r="C461" t="s">
+        <v>422</v>
+      </c>
+      <c r="D461" t="s">
+        <v>340</v>
+      </c>
+      <c r="E461" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="462" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A462" t="s">
+        <v>558</v>
+      </c>
+      <c r="B462" t="s">
+        <v>553</v>
+      </c>
+      <c r="C462" t="s">
+        <v>422</v>
+      </c>
+      <c r="D462" t="s">
+        <v>340</v>
+      </c>
+      <c r="E462" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="463" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A463" t="s">
+        <v>560</v>
+      </c>
+      <c r="B463" t="s">
+        <v>561</v>
+      </c>
+      <c r="C463" t="s">
+        <v>350</v>
+      </c>
+      <c r="D463" t="s">
+        <v>340</v>
+      </c>
+      <c r="E463" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="464" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A464" t="s">
+        <v>560</v>
+      </c>
+      <c r="B464" t="s">
+        <v>562</v>
+      </c>
+      <c r="C464" t="s">
+        <v>350</v>
+      </c>
+      <c r="D464" t="s">
+        <v>340</v>
+      </c>
+      <c r="E464" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="465" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A465" t="s">
+        <v>560</v>
+      </c>
+      <c r="B465" t="s">
+        <v>563</v>
+      </c>
+      <c r="C465" t="s">
+        <v>350</v>
+      </c>
+      <c r="D465" t="s">
+        <v>340</v>
+      </c>
+      <c r="E465" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="466" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A466" t="s">
+        <v>560</v>
+      </c>
+      <c r="B466" t="s">
+        <v>564</v>
+      </c>
+      <c r="C466" t="s">
+        <v>350</v>
+      </c>
+      <c r="D466" t="s">
+        <v>340</v>
+      </c>
+      <c r="E466" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="467" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A467" t="s">
+        <v>560</v>
+      </c>
+      <c r="B467" t="s">
+        <v>565</v>
+      </c>
+      <c r="C467" t="s">
+        <v>350</v>
+      </c>
+      <c r="D467" t="s">
+        <v>340</v>
+      </c>
+      <c r="E467" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="468" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A468" t="s">
+        <v>560</v>
+      </c>
+      <c r="B468" t="s">
+        <v>566</v>
+      </c>
+      <c r="C468" t="s">
+        <v>350</v>
+      </c>
+      <c r="D468" t="s">
+        <v>340</v>
+      </c>
+      <c r="E468" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="469" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A469" t="s">
+        <v>560</v>
+      </c>
+      <c r="B469" t="s">
+        <v>567</v>
+      </c>
+      <c r="C469" t="s">
+        <v>350</v>
+      </c>
+      <c r="D469" t="s">
+        <v>340</v>
+      </c>
+      <c r="E469" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="470" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A470" t="s">
+        <v>560</v>
+      </c>
+      <c r="B470" t="s">
+        <v>568</v>
+      </c>
+      <c r="C470" t="s">
+        <v>350</v>
+      </c>
+      <c r="D470" t="s">
+        <v>340</v>
+      </c>
+      <c r="E470" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="471" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A471" t="s">
+        <v>560</v>
+      </c>
+      <c r="B471" t="s">
+        <v>569</v>
+      </c>
+      <c r="C471" t="s">
+        <v>350</v>
+      </c>
+      <c r="D471" t="s">
+        <v>340</v>
+      </c>
+      <c r="E471" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="472" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A472" t="s">
+        <v>560</v>
+      </c>
+      <c r="B472" t="s">
+        <v>559</v>
+      </c>
+      <c r="C472" t="s">
+        <v>350</v>
+      </c>
+      <c r="D472" t="s">
+        <v>340</v>
+      </c>
+      <c r="E472" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="473" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A473" t="s">
+        <v>570</v>
+      </c>
+      <c r="B473" t="s">
+        <v>572</v>
+      </c>
+      <c r="C473" t="s">
+        <v>463</v>
+      </c>
+      <c r="D473" t="s">
+        <v>340</v>
+      </c>
+      <c r="E473" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="474" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A474" t="s">
+        <v>570</v>
+      </c>
+      <c r="B474" t="s">
+        <v>571</v>
+      </c>
+      <c r="C474" t="s">
+        <v>463</v>
+      </c>
+      <c r="D474" t="s">
+        <v>340</v>
+      </c>
+      <c r="E474" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="475" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A475" t="s">
+        <v>573</v>
+      </c>
+      <c r="B475" t="s">
+        <v>576</v>
+      </c>
+      <c r="C475" t="s">
+        <v>575</v>
+      </c>
+      <c r="D475" t="s">
+        <v>340</v>
+      </c>
+      <c r="E475" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="476" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A476" t="s">
+        <v>573</v>
+      </c>
+      <c r="B476" t="s">
+        <v>577</v>
+      </c>
+      <c r="C476" t="s">
+        <v>575</v>
+      </c>
+      <c r="D476" t="s">
+        <v>340</v>
+      </c>
+      <c r="E476" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="477" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A477" t="s">
+        <v>573</v>
+      </c>
+      <c r="B477" t="s">
+        <v>578</v>
+      </c>
+      <c r="C477" t="s">
+        <v>575</v>
+      </c>
+      <c r="D477" t="s">
+        <v>340</v>
+      </c>
+      <c r="E477" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="478" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A478" t="s">
+        <v>573</v>
+      </c>
+      <c r="B478" t="s">
+        <v>579</v>
+      </c>
+      <c r="C478" t="s">
+        <v>575</v>
+      </c>
+      <c r="D478" t="s">
+        <v>340</v>
+      </c>
+      <c r="E478" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="479" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A479" t="s">
+        <v>573</v>
+      </c>
+      <c r="B479" t="s">
+        <v>580</v>
+      </c>
+      <c r="C479" t="s">
+        <v>575</v>
+      </c>
+      <c r="D479" t="s">
+        <v>340</v>
+      </c>
+      <c r="E479" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="480" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A480" t="s">
+        <v>573</v>
+      </c>
+      <c r="B480" t="s">
+        <v>581</v>
+      </c>
+      <c r="C480" t="s">
+        <v>575</v>
+      </c>
+      <c r="D480" t="s">
+        <v>340</v>
+      </c>
+      <c r="E480" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="481" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A481" t="s">
+        <v>573</v>
+      </c>
+      <c r="B481" t="s">
+        <v>582</v>
+      </c>
+      <c r="C481" t="s">
+        <v>575</v>
+      </c>
+      <c r="D481" t="s">
+        <v>340</v>
+      </c>
+      <c r="E481" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="482" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A482" t="s">
+        <v>573</v>
+      </c>
+      <c r="B482" t="s">
+        <v>574</v>
+      </c>
+      <c r="C482" t="s">
+        <v>575</v>
+      </c>
+      <c r="D482" t="s">
+        <v>340</v>
+      </c>
+      <c r="E482" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="483" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A483" t="s">
+        <v>583</v>
+      </c>
+      <c r="B483" t="s">
+        <v>584</v>
+      </c>
+      <c r="C483" t="s">
+        <v>350</v>
+      </c>
+      <c r="D483" t="s">
+        <v>340</v>
+      </c>
+      <c r="E483" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="484" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A484" t="s">
+        <v>583</v>
+      </c>
+      <c r="B484" t="s">
+        <v>585</v>
+      </c>
+      <c r="C484" t="s">
+        <v>350</v>
+      </c>
+      <c r="D484" t="s">
+        <v>340</v>
+      </c>
+      <c r="E484" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="485" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A485" t="s">
+        <v>583</v>
+      </c>
+      <c r="B485" t="s">
+        <v>586</v>
+      </c>
+      <c r="C485" t="s">
+        <v>350</v>
+      </c>
+      <c r="D485" t="s">
+        <v>340</v>
+      </c>
+      <c r="E485" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="486" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A486" t="s">
+        <v>583</v>
+      </c>
+      <c r="B486" t="s">
+        <v>587</v>
+      </c>
+      <c r="C486" t="s">
+        <v>350</v>
+      </c>
+      <c r="D486" t="s">
+        <v>340</v>
+      </c>
+      <c r="E486" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="487" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A487" t="s">
+        <v>589</v>
+      </c>
+      <c r="B487" t="s">
+        <v>590</v>
+      </c>
+      <c r="C487" t="s">
+        <v>593</v>
+      </c>
+      <c r="D487" t="s">
+        <v>340</v>
+      </c>
+      <c r="E487" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="488" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A488" t="s">
+        <v>589</v>
+      </c>
+      <c r="B488" t="s">
+        <v>591</v>
+      </c>
+      <c r="C488" t="s">
+        <v>593</v>
+      </c>
+      <c r="D488" t="s">
+        <v>340</v>
+      </c>
+      <c r="E488" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="489" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A489" t="s">
+        <v>589</v>
+      </c>
+      <c r="B489" t="s">
+        <v>592</v>
+      </c>
+      <c r="C489" t="s">
+        <v>593</v>
+      </c>
+      <c r="D489" t="s">
+        <v>340</v>
+      </c>
+      <c r="E489" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="490" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A490" t="s">
+        <v>589</v>
+      </c>
+      <c r="B490" t="s">
+        <v>588</v>
+      </c>
+      <c r="C490" t="s">
+        <v>593</v>
+      </c>
+      <c r="D490" t="s">
+        <v>340</v>
+      </c>
+      <c r="E490" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="491" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A491" t="s">
+        <v>594</v>
+      </c>
+      <c r="B491" t="s">
+        <v>595</v>
+      </c>
+      <c r="C491" t="s">
+        <v>593</v>
+      </c>
+      <c r="D491" t="s">
+        <v>340</v>
+      </c>
+      <c r="E491" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="492" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A492" t="s">
+        <v>594</v>
+      </c>
+      <c r="B492" t="s">
+        <v>596</v>
+      </c>
+      <c r="C492" t="s">
+        <v>593</v>
+      </c>
+      <c r="D492" t="s">
+        <v>340</v>
+      </c>
+      <c r="E492" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="493" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A493" t="s">
+        <v>594</v>
+      </c>
+      <c r="B493" t="s">
+        <v>597</v>
+      </c>
+      <c r="C493" t="s">
+        <v>593</v>
+      </c>
+      <c r="D493" t="s">
+        <v>340</v>
+      </c>
+      <c r="E493" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="494" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A494" t="s">
+        <v>594</v>
+      </c>
+      <c r="B494" t="s">
+        <v>598</v>
+      </c>
+      <c r="C494" t="s">
+        <v>593</v>
+      </c>
+      <c r="D494" t="s">
+        <v>340</v>
+      </c>
+      <c r="E494" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="495" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A495" t="s">
+        <v>594</v>
+      </c>
+      <c r="B495" t="s">
+        <v>599</v>
+      </c>
+      <c r="C495" t="s">
+        <v>593</v>
+      </c>
+      <c r="D495" t="s">
+        <v>340</v>
+      </c>
+      <c r="E495" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="496" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A496" t="s">
+        <v>594</v>
+      </c>
+      <c r="B496" t="s">
+        <v>600</v>
+      </c>
+      <c r="C496" t="s">
+        <v>593</v>
+      </c>
+      <c r="D496" t="s">
+        <v>340</v>
+      </c>
+      <c r="E496" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="497" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A497" t="s">
+        <v>594</v>
+      </c>
+      <c r="B497" t="s">
+        <v>601</v>
+      </c>
+      <c r="C497" t="s">
+        <v>593</v>
+      </c>
+      <c r="D497" t="s">
+        <v>340</v>
+      </c>
+      <c r="E497" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="498" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A498" t="s">
+        <v>594</v>
+      </c>
+      <c r="B498" t="s">
+        <v>602</v>
+      </c>
+      <c r="C498" t="s">
+        <v>593</v>
+      </c>
+      <c r="D498" t="s">
+        <v>340</v>
+      </c>
+      <c r="E498" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="499" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A499" t="s">
+        <v>594</v>
+      </c>
+      <c r="B499" t="s">
+        <v>603</v>
+      </c>
+      <c r="C499" t="s">
+        <v>593</v>
+      </c>
+      <c r="D499" t="s">
+        <v>340</v>
+      </c>
+      <c r="E499" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="500" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A500" t="s">
+        <v>604</v>
+      </c>
+      <c r="B500" t="s">
+        <v>606</v>
+      </c>
+      <c r="C500" t="s">
+        <v>593</v>
+      </c>
+      <c r="D500" t="s">
+        <v>340</v>
+      </c>
+      <c r="E500" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="501" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A501" t="s">
+        <v>604</v>
+      </c>
+      <c r="B501" t="s">
+        <v>607</v>
+      </c>
+      <c r="C501" t="s">
+        <v>593</v>
+      </c>
+      <c r="D501" t="s">
+        <v>340</v>
+      </c>
+      <c r="E501" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="502" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A502" t="s">
+        <v>604</v>
+      </c>
+      <c r="B502" t="s">
+        <v>608</v>
+      </c>
+      <c r="C502" t="s">
+        <v>593</v>
+      </c>
+      <c r="D502" t="s">
+        <v>340</v>
+      </c>
+      <c r="E502" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="503" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A503" t="s">
+        <v>604</v>
+      </c>
+      <c r="B503" t="s">
+        <v>609</v>
+      </c>
+      <c r="C503" t="s">
+        <v>593</v>
+      </c>
+      <c r="D503" t="s">
+        <v>340</v>
+      </c>
+      <c r="E503" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="504" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A504" t="s">
+        <v>604</v>
+      </c>
+      <c r="B504" t="s">
+        <v>610</v>
+      </c>
+      <c r="C504" t="s">
+        <v>593</v>
+      </c>
+      <c r="D504" t="s">
+        <v>340</v>
+      </c>
+      <c r="E504" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="505" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A505" t="s">
+        <v>604</v>
+      </c>
+      <c r="B505" t="s">
+        <v>611</v>
+      </c>
+      <c r="C505" t="s">
+        <v>593</v>
+      </c>
+      <c r="D505" t="s">
+        <v>340</v>
+      </c>
+      <c r="E505" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="506" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A506" t="s">
+        <v>604</v>
+      </c>
+      <c r="B506" t="s">
+        <v>612</v>
+      </c>
+      <c r="C506" t="s">
+        <v>593</v>
+      </c>
+      <c r="D506" t="s">
+        <v>340</v>
+      </c>
+      <c r="E506" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="507" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A507" t="s">
+        <v>604</v>
+      </c>
+      <c r="B507" t="s">
+        <v>613</v>
+      </c>
+      <c r="C507" t="s">
+        <v>593</v>
+      </c>
+      <c r="D507" t="s">
+        <v>340</v>
+      </c>
+      <c r="E507" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="508" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A508" t="s">
+        <v>604</v>
+      </c>
+      <c r="B508" t="s">
+        <v>614</v>
+      </c>
+      <c r="C508" t="s">
+        <v>593</v>
+      </c>
+      <c r="D508" t="s">
+        <v>340</v>
+      </c>
+      <c r="E508" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="509" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A509" t="s">
+        <v>604</v>
+      </c>
+      <c r="B509" t="s">
+        <v>615</v>
+      </c>
+      <c r="C509" t="s">
+        <v>593</v>
+      </c>
+      <c r="D509" t="s">
+        <v>340</v>
+      </c>
+      <c r="E509" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="510" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A510" t="s">
+        <v>604</v>
+      </c>
+      <c r="B510" t="s">
+        <v>616</v>
+      </c>
+      <c r="C510" t="s">
+        <v>593</v>
+      </c>
+      <c r="D510" t="s">
+        <v>340</v>
+      </c>
+      <c r="E510" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="511" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A511" t="s">
+        <v>604</v>
+      </c>
+      <c r="B511" t="s">
+        <v>617</v>
+      </c>
+      <c r="C511" t="s">
+        <v>593</v>
+      </c>
+      <c r="D511" t="s">
+        <v>340</v>
+      </c>
+      <c r="E511" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="512" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A512" t="s">
+        <v>604</v>
+      </c>
+      <c r="B512" t="s">
+        <v>605</v>
+      </c>
+      <c r="C512" t="s">
+        <v>593</v>
+      </c>
+      <c r="D512" t="s">
+        <v>340</v>
+      </c>
+      <c r="E512" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="513" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A513" t="s">
+        <v>618</v>
+      </c>
+      <c r="B513" t="s">
+        <v>620</v>
+      </c>
+      <c r="C513" t="s">
+        <v>350</v>
+      </c>
+      <c r="D513" t="s">
+        <v>340</v>
+      </c>
+      <c r="E513" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="514" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A514" t="s">
+        <v>618</v>
+      </c>
+      <c r="B514" t="s">
+        <v>621</v>
+      </c>
+      <c r="C514" t="s">
+        <v>350</v>
+      </c>
+      <c r="D514" t="s">
+        <v>340</v>
+      </c>
+      <c r="E514" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="515" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A515" t="s">
+        <v>618</v>
+      </c>
+      <c r="B515" t="s">
+        <v>622</v>
+      </c>
+      <c r="C515" t="s">
+        <v>350</v>
+      </c>
+      <c r="D515" t="s">
+        <v>340</v>
+      </c>
+      <c r="E515" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="516" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A516" t="s">
+        <v>618</v>
+      </c>
+      <c r="B516" t="s">
+        <v>623</v>
+      </c>
+      <c r="C516" t="s">
+        <v>350</v>
+      </c>
+      <c r="D516" t="s">
+        <v>340</v>
+      </c>
+      <c r="E516" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="517" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A517" t="s">
+        <v>618</v>
+      </c>
+      <c r="B517" t="s">
+        <v>624</v>
+      </c>
+      <c r="C517" t="s">
+        <v>350</v>
+      </c>
+      <c r="D517" t="s">
+        <v>340</v>
+      </c>
+      <c r="E517" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="518" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A518" t="s">
+        <v>618</v>
+      </c>
+      <c r="B518" t="s">
+        <v>625</v>
+      </c>
+      <c r="C518" t="s">
+        <v>350</v>
+      </c>
+      <c r="D518" t="s">
+        <v>340</v>
+      </c>
+      <c r="E518" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="519" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A519" t="s">
+        <v>618</v>
+      </c>
+      <c r="B519" t="s">
+        <v>619</v>
+      </c>
+      <c r="C519" t="s">
+        <v>350</v>
+      </c>
+      <c r="D519" t="s">
+        <v>340</v>
+      </c>
+      <c r="E519" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="520" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A520" t="s">
+        <v>626</v>
+      </c>
+      <c r="B520" t="s">
+        <v>628</v>
+      </c>
+      <c r="C520" t="s">
+        <v>593</v>
+      </c>
+      <c r="D520" t="s">
+        <v>340</v>
+      </c>
+      <c r="E520" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="521" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A521" t="s">
+        <v>629</v>
+      </c>
+      <c r="B521" t="s">
+        <v>630</v>
+      </c>
+      <c r="C521" t="s">
+        <v>593</v>
+      </c>
+      <c r="D521" t="s">
+        <v>340</v>
+      </c>
+      <c r="E521" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="522" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A522" t="s">
+        <v>632</v>
+      </c>
+      <c r="B522" t="s">
+        <v>631</v>
+      </c>
+      <c r="C522" t="s">
+        <v>593</v>
+      </c>
+      <c r="D522" t="s">
+        <v>340</v>
+      </c>
+      <c r="E522" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="523" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A523" t="s">
+        <v>632</v>
+      </c>
+      <c r="B523" t="s">
+        <v>633</v>
+      </c>
+      <c r="C523" t="s">
+        <v>593</v>
+      </c>
+      <c r="D523" t="s">
+        <v>340</v>
+      </c>
+      <c r="E523" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="524" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A524" t="s">
+        <v>626</v>
+      </c>
+      <c r="B524" t="s">
+        <v>634</v>
+      </c>
+      <c r="C524" t="s">
+        <v>593</v>
+      </c>
+      <c r="D524" t="s">
+        <v>340</v>
+      </c>
+      <c r="E524" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="525" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A525" t="s">
+        <v>626</v>
+      </c>
+      <c r="B525" t="s">
+        <v>627</v>
+      </c>
+      <c r="C525" t="s">
+        <v>593</v>
+      </c>
+      <c r="D525" t="s">
+        <v>340</v>
+      </c>
+      <c r="E525" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="526" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A526" t="s">
+        <v>635</v>
+      </c>
+      <c r="B526" t="s">
+        <v>635</v>
+      </c>
+      <c r="C526" t="s">
+        <v>516</v>
+      </c>
+      <c r="D526" t="s">
+        <v>340</v>
+      </c>
+      <c r="E526" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="527" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A527" t="s">
+        <v>635</v>
+      </c>
+      <c r="B527" t="s">
+        <v>636</v>
+      </c>
+      <c r="C527" t="s">
+        <v>516</v>
+      </c>
+      <c r="D527" t="s">
+        <v>340</v>
+      </c>
+      <c r="E527" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="528" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A528" t="s">
+        <v>635</v>
+      </c>
+      <c r="B528" t="s">
+        <v>637</v>
+      </c>
+      <c r="C528" t="s">
+        <v>516</v>
+      </c>
+      <c r="D528" t="s">
+        <v>340</v>
+      </c>
+      <c r="E528" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="529" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A529" t="s">
+        <v>635</v>
+      </c>
+      <c r="B529" t="s">
+        <v>638</v>
+      </c>
+      <c r="C529" t="s">
+        <v>516</v>
+      </c>
+      <c r="D529" t="s">
+        <v>340</v>
+      </c>
+      <c r="E529" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="530" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A530" t="s">
+        <v>635</v>
+      </c>
+      <c r="B530" t="s">
+        <v>639</v>
+      </c>
+      <c r="C530" t="s">
+        <v>516</v>
+      </c>
+      <c r="D530" t="s">
+        <v>340</v>
+      </c>
+      <c r="E530" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="531" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A531" t="s">
+        <v>635</v>
+      </c>
+      <c r="B531" t="s">
+        <v>640</v>
+      </c>
+      <c r="C531" t="s">
+        <v>516</v>
+      </c>
+      <c r="D531" t="s">
+        <v>340</v>
+      </c>
+      <c r="E531" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="532" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A532" t="s">
+        <v>635</v>
+      </c>
+      <c r="B532" t="s">
+        <v>641</v>
+      </c>
+      <c r="C532" t="s">
+        <v>516</v>
+      </c>
+      <c r="D532" t="s">
+        <v>340</v>
+      </c>
+      <c r="E532" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="533" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A533" t="s">
+        <v>635</v>
+      </c>
+      <c r="B533" t="s">
+        <v>642</v>
+      </c>
+      <c r="C533" t="s">
+        <v>516</v>
+      </c>
+      <c r="D533" t="s">
+        <v>340</v>
+      </c>
+      <c r="E533" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="534" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A534" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="535" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A535" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="536" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A536" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="537" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A537" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="538" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A538" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="539" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A539" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="540" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A540" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="541" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A541" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="542" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A542" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="543" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A543" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="544" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A544" t="s">
+        <v>653</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
completed list of albums. downloaded json files for each album in list. added general outline of project to readme.
</commit_message>
<xml_diff>
--- a/album_list.xlsx
+++ b/album_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP USER\Coding\Play\Rap_Lyrics\lyricsNLP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E115D4CA-FFE2-4E38-97F3-3AED5EC15C60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F90F178-D165-4D0C-8480-CB7416C57DF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4CD478C6-4722-4BC8-838A-CC153C60C18A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4347" uniqueCount="1058">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5353" uniqueCount="1280">
   <si>
     <t>Artist</t>
   </si>
@@ -3210,6 +3210,672 @@
   </si>
   <si>
     <t>DJ Quik</t>
+  </si>
+  <si>
+    <t>Mos Def</t>
+  </si>
+  <si>
+    <t>Talib Kweli</t>
+  </si>
+  <si>
+    <t>Arrested Development</t>
+  </si>
+  <si>
+    <t>Coast Contra</t>
+  </si>
+  <si>
+    <t>Afroman</t>
+  </si>
+  <si>
+    <t>Childish Gambino</t>
+  </si>
+  <si>
+    <t>Lil Dicky</t>
+  </si>
+  <si>
+    <t>The Cool Kids</t>
+  </si>
+  <si>
+    <t>Del The Funky Homosapien</t>
+  </si>
+  <si>
+    <t>A$AP Rocky</t>
+  </si>
+  <si>
+    <t>Goldlink</t>
+  </si>
+  <si>
+    <t>Action Bronson</t>
+  </si>
+  <si>
+    <t>Jurassic 5</t>
+  </si>
+  <si>
+    <t>Raekwon</t>
+  </si>
+  <si>
+    <t>People Under the Stairs</t>
+  </si>
+  <si>
+    <t>Victory Lap</t>
+  </si>
+  <si>
+    <t>The Marathon</t>
+  </si>
+  <si>
+    <t>The Marathon Continues</t>
+  </si>
+  <si>
+    <t>Crenshaw</t>
+  </si>
+  <si>
+    <t>Mailbox Money</t>
+  </si>
+  <si>
+    <t>Slauson Boy 2</t>
+  </si>
+  <si>
+    <t>Drillmatic – Heart vs. Mind</t>
+  </si>
+  <si>
+    <t>Untold Story</t>
+  </si>
+  <si>
+    <t>The Documentary</t>
+  </si>
+  <si>
+    <t>Doctor's Advocate</t>
+  </si>
+  <si>
+    <t>LAX</t>
+  </si>
+  <si>
+    <t>The R.E.D. Album</t>
+  </si>
+  <si>
+    <t>Jesus Piece</t>
+  </si>
+  <si>
+    <t>The Documentary 2</t>
+  </si>
+  <si>
+    <t>The Documentary 2.5</t>
+  </si>
+  <si>
+    <t>Born 2 Rap</t>
+  </si>
+  <si>
+    <t>Napalm</t>
+  </si>
+  <si>
+    <t>At the Speed of Life</t>
+  </si>
+  <si>
+    <t>40 Dayz &amp; 40 Nightz</t>
+  </si>
+  <si>
+    <t>Restless</t>
+  </si>
+  <si>
+    <t>Man vs. Machine</t>
+  </si>
+  <si>
+    <t>Weapons of Mass Destruction</t>
+  </si>
+  <si>
+    <t>Full Circle</t>
+  </si>
+  <si>
+    <t>High Maintenance</t>
+  </si>
+  <si>
+    <t>Icy</t>
+  </si>
+  <si>
+    <t>Pretty Summer Playlist: Season 1</t>
+  </si>
+  <si>
+    <t>Ramona Park Broke My Heart</t>
+  </si>
+  <si>
+    <t>Summertime '06</t>
+  </si>
+  <si>
+    <t>Big Fish Theory</t>
+  </si>
+  <si>
+    <t>FM!</t>
+  </si>
+  <si>
+    <t>Call Me If You Get Lost</t>
+  </si>
+  <si>
+    <t>Goblin</t>
+  </si>
+  <si>
+    <t>Wolf</t>
+  </si>
+  <si>
+    <t>Cherry Bomb</t>
+  </si>
+  <si>
+    <t>Flower Boy</t>
+  </si>
+  <si>
+    <t>Igor</t>
+  </si>
+  <si>
+    <t>The G Files</t>
+  </si>
+  <si>
+    <t>Regulate... G Funk Era</t>
+  </si>
+  <si>
+    <t>Take a Look Over Your Shoulder</t>
+  </si>
+  <si>
+    <t>I Want It All</t>
+  </si>
+  <si>
+    <t>The Return of the Regulator</t>
+  </si>
+  <si>
+    <t>In the Mid-Nite Hour</t>
+  </si>
+  <si>
+    <t>Follow Me Home</t>
+  </si>
+  <si>
+    <t>Redemption</t>
+  </si>
+  <si>
+    <t>DanceJamtheMusic</t>
+  </si>
+  <si>
+    <t>Feel My Power</t>
+  </si>
+  <si>
+    <t>Let's Get It Started</t>
+  </si>
+  <si>
+    <t>Please Hammer Don't Hurt 'Em</t>
+  </si>
+  <si>
+    <t>Too Legit to Quit</t>
+  </si>
+  <si>
+    <t>The Funky Headhunter</t>
+  </si>
+  <si>
+    <t>Inside Out</t>
+  </si>
+  <si>
+    <t>Family Affair</t>
+  </si>
+  <si>
+    <t>Active Duty</t>
+  </si>
+  <si>
+    <t>Full Blast</t>
+  </si>
+  <si>
+    <t>Look Look Look</t>
+  </si>
+  <si>
+    <t>Live Life Fast</t>
+  </si>
+  <si>
+    <t>Please Excuse Me for Being Antisocial</t>
+  </si>
+  <si>
+    <t>The Midnight Life</t>
+  </si>
+  <si>
+    <t>Quik Is the Name</t>
+  </si>
+  <si>
+    <t>Way 2 Fonky</t>
+  </si>
+  <si>
+    <t>Safe + Sound</t>
+  </si>
+  <si>
+    <t>Rhythm-al-ism</t>
+  </si>
+  <si>
+    <t>Balance &amp; Options</t>
+  </si>
+  <si>
+    <t>Under tha Influence</t>
+  </si>
+  <si>
+    <t>Trauma</t>
+  </si>
+  <si>
+    <t>The Book of David</t>
+  </si>
+  <si>
+    <t>Crash Talk</t>
+  </si>
+  <si>
+    <t>Setbacks</t>
+  </si>
+  <si>
+    <t>Habits &amp; Contradictions</t>
+  </si>
+  <si>
+    <t>Oxymoron</t>
+  </si>
+  <si>
+    <t>Blank Face LP</t>
+  </si>
+  <si>
+    <t>The Ecstatic</t>
+  </si>
+  <si>
+    <t>Black on Both Sides</t>
+  </si>
+  <si>
+    <t>The New Danger</t>
+  </si>
+  <si>
+    <t>True Magic</t>
+  </si>
+  <si>
+    <t>Radio Silence</t>
+  </si>
+  <si>
+    <t>Quality</t>
+  </si>
+  <si>
+    <t>The Beautiful Struggle</t>
+  </si>
+  <si>
+    <t>Eardrum</t>
+  </si>
+  <si>
+    <t>Gutter Rainbows</t>
+  </si>
+  <si>
+    <t>Prisoner of Conscious</t>
+  </si>
+  <si>
+    <t>Gravitas</t>
+  </si>
+  <si>
+    <t>Fuck the Money</t>
+  </si>
+  <si>
+    <t>When Fish Ride Bicycles</t>
+  </si>
+  <si>
+    <t>Special Edition Grand Master Deluxe</t>
+  </si>
+  <si>
+    <t>Volumes</t>
+  </si>
+  <si>
+    <t>Before Shit Got Weird</t>
+  </si>
+  <si>
+    <t>The Bake Sale</t>
+  </si>
+  <si>
+    <t>3 Years, 5 Months and 2 Days in the Life Of…</t>
+  </si>
+  <si>
+    <t>Unplugged</t>
+  </si>
+  <si>
+    <t>Zingalamaduni</t>
+  </si>
+  <si>
+    <t>Da Feelin' EP</t>
+  </si>
+  <si>
+    <t>Heroes of the Harvest</t>
+  </si>
+  <si>
+    <t>Extended Revolution</t>
+  </si>
+  <si>
+    <t>Among the Trees</t>
+  </si>
+  <si>
+    <t>Since the Last Time</t>
+  </si>
+  <si>
+    <t>Strong</t>
+  </si>
+  <si>
+    <t>Standing at the Crossroads</t>
+  </si>
+  <si>
+    <t>Changing The Narrative</t>
+  </si>
+  <si>
+    <t>This Was Never Home</t>
+  </si>
+  <si>
+    <t>Craft &amp; Optics</t>
+  </si>
+  <si>
+    <t>Don't Fight Your Demons</t>
+  </si>
+  <si>
+    <t>For the Fkn Love</t>
+  </si>
+  <si>
+    <t>Apt. 505</t>
+  </si>
+  <si>
+    <t>Palmdale</t>
+  </si>
+  <si>
+    <t>Lemon Pound Cake</t>
+  </si>
+  <si>
+    <t>My Fro-losophy</t>
+  </si>
+  <si>
+    <t>Because I Got High</t>
+  </si>
+  <si>
+    <t>Sell Your Dope</t>
+  </si>
+  <si>
+    <t>The Good Times</t>
+  </si>
+  <si>
+    <t>Afroholic... The Even Better Times</t>
+  </si>
+  <si>
+    <t>Jobe Bells</t>
+  </si>
+  <si>
+    <t>4R0:20</t>
+  </si>
+  <si>
+    <t>The Hungry Hustlerz: Starvation Is Motivation</t>
+  </si>
+  <si>
+    <t>Drunk 'n' High</t>
+  </si>
+  <si>
+    <t>A Colt 45 Christmas</t>
+  </si>
+  <si>
+    <t>Waiting to Inhale</t>
+  </si>
+  <si>
+    <t>Frobama: Head of State</t>
+  </si>
+  <si>
+    <t>Marijuana Music</t>
+  </si>
+  <si>
+    <t>The Frorider</t>
+  </si>
+  <si>
+    <t>Happy to Be Alive</t>
+  </si>
+  <si>
+    <t>Cold Fro-T-5 and Two Frigg Fraggs</t>
+  </si>
+  <si>
+    <t>Save a Cadillac, Ride a Homeboy</t>
+  </si>
+  <si>
+    <t>Camp</t>
+  </si>
+  <si>
+    <t>Because the Internet</t>
+  </si>
+  <si>
+    <t>"Awaken, My Love!"</t>
+  </si>
+  <si>
+    <t>3.15.20</t>
+  </si>
+  <si>
+    <t>Summer Pack</t>
+  </si>
+  <si>
+    <t>STN MTN / Kauai</t>
+  </si>
+  <si>
+    <t>EP</t>
+  </si>
+  <si>
+    <t>Professional Rapper</t>
+  </si>
+  <si>
+    <t>So Hard</t>
+  </si>
+  <si>
+    <t>Hump Days</t>
+  </si>
+  <si>
+    <t>Souls of Mischief</t>
+  </si>
+  <si>
+    <t>Iller Than Most</t>
+  </si>
+  <si>
+    <t>I Wish My Brother George Was Here</t>
+  </si>
+  <si>
+    <t>No Need for Alarm</t>
+  </si>
+  <si>
+    <t>Future Development</t>
+  </si>
+  <si>
+    <t>Both Sides of the Brain</t>
+  </si>
+  <si>
+    <t>Eleventh Hour</t>
+  </si>
+  <si>
+    <t>Funk Man (The Stimulus Package)</t>
+  </si>
+  <si>
+    <t>Automatik Statik</t>
+  </si>
+  <si>
+    <t>It Ain't Illegal Yet</t>
+  </si>
+  <si>
+    <t>Golden Era</t>
+  </si>
+  <si>
+    <t>Root Stimulation</t>
+  </si>
+  <si>
+    <t>Cypress Hill</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Long. Live. A$AP</t>
+  </si>
+  <si>
+    <t>At. Long. Last. A$AP</t>
+  </si>
+  <si>
+    <t>At What Cost</t>
+  </si>
+  <si>
+    <t>Diaspora</t>
+  </si>
+  <si>
+    <t>Haram!</t>
+  </si>
+  <si>
+    <t>Dr. Lecter</t>
+  </si>
+  <si>
+    <t>Mr. Wonderful</t>
+  </si>
+  <si>
+    <t>Blue Chips 7000</t>
+  </si>
+  <si>
+    <t>White Bronco</t>
+  </si>
+  <si>
+    <t>Only for Dolphins</t>
+  </si>
+  <si>
+    <t>Quality Control</t>
+  </si>
+  <si>
+    <t>Power in Numbers</t>
+  </si>
+  <si>
+    <t>Feedback</t>
+  </si>
+  <si>
+    <t>Jurassic 6</t>
+  </si>
+  <si>
+    <t>Jurassic 7</t>
+  </si>
+  <si>
+    <t>Jurassic 8</t>
+  </si>
+  <si>
+    <t>The Wild</t>
+  </si>
+  <si>
+    <t>Only Built 4 Cuban Linx…</t>
+  </si>
+  <si>
+    <t>Immobilarity</t>
+  </si>
+  <si>
+    <t>The Lex Diamond Story</t>
+  </si>
+  <si>
+    <t>Only Built 4 Cuban Linx... Pt. II</t>
+  </si>
+  <si>
+    <t>Shaolin vs. Wu-Tang</t>
+  </si>
+  <si>
+    <t>Fly International Luxurious Art</t>
+  </si>
+  <si>
+    <t>Anderson .Paak</t>
+  </si>
+  <si>
+    <t>Oxnard</t>
+  </si>
+  <si>
+    <t>Ventura</t>
+  </si>
+  <si>
+    <t>Venice</t>
+  </si>
+  <si>
+    <t>Malibu</t>
+  </si>
+  <si>
+    <t>12 Step Program</t>
+  </si>
+  <si>
+    <t>Sincerely, The P</t>
+  </si>
+  <si>
+    <t>The Next Step</t>
+  </si>
+  <si>
+    <t>Question in the Form of an Answer</t>
+  </si>
+  <si>
+    <t>O.S.T.</t>
+  </si>
+  <si>
+    <t>...Or Stay Tuned</t>
+  </si>
+  <si>
+    <t>Stepfather</t>
+  </si>
+  <si>
+    <t>Fun DMC</t>
+  </si>
+  <si>
+    <t>Carried Away</t>
+  </si>
+  <si>
+    <t>Highlighter</t>
+  </si>
+  <si>
+    <t>The Gettin' Off Stage, Step 1</t>
+  </si>
+  <si>
+    <t>The Gettin' Off Stage, Step 2</t>
+  </si>
+  <si>
+    <t>The Pharcyde</t>
+  </si>
+  <si>
+    <t>Bizarre Ride II the Pharcyde</t>
+  </si>
+  <si>
+    <t>Labcabincalifornia</t>
+  </si>
+  <si>
+    <t>Plain Rap</t>
+  </si>
+  <si>
+    <t>Humboldt Beginnings</t>
+  </si>
+  <si>
+    <t>93 'til Infinity</t>
+  </si>
+  <si>
+    <t>No Man's Land</t>
+  </si>
+  <si>
+    <t>Focus</t>
+  </si>
+  <si>
+    <t>Trilogy: Conflict, Climax, Resolution</t>
+  </si>
+  <si>
+    <t>Montezuma's Revenge</t>
+  </si>
+  <si>
+    <t>There Is Only Now</t>
+  </si>
+  <si>
+    <t>South Gate</t>
+  </si>
+  <si>
+    <t>Back in Black</t>
+  </si>
+  <si>
+    <t>Black Sunday</t>
+  </si>
+  <si>
+    <t>III: Temples of Boom</t>
+  </si>
+  <si>
+    <t>IV</t>
+  </si>
+  <si>
+    <t>Skull &amp; Bones</t>
+  </si>
+  <si>
+    <t>Stoned Raiders</t>
+  </si>
+  <si>
+    <t>Rise Up</t>
+  </si>
+  <si>
+    <t>Elephants on Acid</t>
   </si>
 </sst>
 </file>
@@ -3604,10 +4270,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71A19CDE-E3DD-497E-8468-EF613F78BA90}">
-  <dimension ref="A1:E881"/>
+  <dimension ref="A1:E1073"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A861" workbookViewId="0">
-      <selection activeCell="A882" sqref="A882"/>
+    <sheetView tabSelected="1" topLeftCell="A1051" workbookViewId="0">
+      <selection activeCell="G1067" sqref="G1067"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16621,7 +17287,7 @@
         <v>933</v>
       </c>
       <c r="C766" t="s">
-        <v>876</v>
+        <v>946</v>
       </c>
       <c r="D766" t="s">
         <v>877</v>
@@ -16638,7 +17304,7 @@
         <v>932</v>
       </c>
       <c r="C767" t="s">
-        <v>876</v>
+        <v>946</v>
       </c>
       <c r="D767" t="s">
         <v>877</v>
@@ -16825,7 +17491,7 @@
         <v>947</v>
       </c>
       <c r="C778" t="s">
-        <v>876</v>
+        <v>946</v>
       </c>
       <c r="D778" t="s">
         <v>877</v>
@@ -16842,7 +17508,7 @@
         <v>2001</v>
       </c>
       <c r="C779" t="s">
-        <v>876</v>
+        <v>946</v>
       </c>
       <c r="D779" t="s">
         <v>877</v>
@@ -16859,7 +17525,7 @@
         <v>946</v>
       </c>
       <c r="C780" t="s">
-        <v>876</v>
+        <v>946</v>
       </c>
       <c r="D780" t="s">
         <v>877</v>
@@ -18304,7 +18970,7 @@
         <v>1042</v>
       </c>
       <c r="C865" t="s">
-        <v>876</v>
+        <v>946</v>
       </c>
       <c r="D865" t="s">
         <v>877</v>
@@ -18321,7 +18987,7 @@
         <v>1043</v>
       </c>
       <c r="C866" t="s">
-        <v>876</v>
+        <v>946</v>
       </c>
       <c r="D866" t="s">
         <v>877</v>
@@ -18338,7 +19004,7 @@
         <v>1044</v>
       </c>
       <c r="C867" t="s">
-        <v>876</v>
+        <v>946</v>
       </c>
       <c r="D867" t="s">
         <v>877</v>
@@ -18355,7 +19021,7 @@
         <v>1045</v>
       </c>
       <c r="C868" t="s">
-        <v>876</v>
+        <v>946</v>
       </c>
       <c r="D868" t="s">
         <v>877</v>
@@ -18372,7 +19038,7 @@
         <v>1041</v>
       </c>
       <c r="C869" t="s">
-        <v>876</v>
+        <v>946</v>
       </c>
       <c r="D869" t="s">
         <v>877</v>
@@ -18385,60 +19051,3468 @@
       <c r="A870" t="s">
         <v>1046</v>
       </c>
+      <c r="B870" t="s">
+        <v>1073</v>
+      </c>
+      <c r="C870" t="s">
+        <v>876</v>
+      </c>
+      <c r="D870" t="s">
+        <v>877</v>
+      </c>
+      <c r="E870" t="s">
+        <v>878</v>
+      </c>
     </row>
     <row r="871" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A871" t="s">
-        <v>1047</v>
+        <v>1046</v>
+      </c>
+      <c r="B871" t="s">
+        <v>1074</v>
+      </c>
+      <c r="C871" t="s">
+        <v>876</v>
+      </c>
+      <c r="D871" t="s">
+        <v>877</v>
+      </c>
+      <c r="E871" t="s">
+        <v>878</v>
       </c>
     </row>
     <row r="872" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A872" t="s">
-        <v>1048</v>
+        <v>1046</v>
+      </c>
+      <c r="B872" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C872" t="s">
+        <v>876</v>
+      </c>
+      <c r="D872" t="s">
+        <v>877</v>
+      </c>
+      <c r="E872" t="s">
+        <v>878</v>
       </c>
     </row>
     <row r="873" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A873" t="s">
-        <v>1049</v>
+        <v>1046</v>
+      </c>
+      <c r="B873" t="s">
+        <v>1076</v>
+      </c>
+      <c r="C873" t="s">
+        <v>876</v>
+      </c>
+      <c r="D873" t="s">
+        <v>877</v>
+      </c>
+      <c r="E873" t="s">
+        <v>878</v>
       </c>
     </row>
     <row r="874" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A874" t="s">
-        <v>1050</v>
+        <v>1046</v>
+      </c>
+      <c r="B874" t="s">
+        <v>1077</v>
+      </c>
+      <c r="C874" t="s">
+        <v>876</v>
+      </c>
+      <c r="D874" t="s">
+        <v>877</v>
+      </c>
+      <c r="E874" t="s">
+        <v>878</v>
       </c>
     </row>
     <row r="875" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A875" t="s">
-        <v>1051</v>
+        <v>1046</v>
+      </c>
+      <c r="B875" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C875" t="s">
+        <v>876</v>
+      </c>
+      <c r="D875" t="s">
+        <v>877</v>
+      </c>
+      <c r="E875" t="s">
+        <v>878</v>
       </c>
     </row>
     <row r="876" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A876" t="s">
-        <v>1052</v>
+        <v>1047</v>
+      </c>
+      <c r="B876" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C876" t="s">
+        <v>946</v>
+      </c>
+      <c r="D876" t="s">
+        <v>877</v>
+      </c>
+      <c r="E876" t="s">
+        <v>878</v>
       </c>
     </row>
     <row r="877" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A877" t="s">
-        <v>1053</v>
+        <v>1047</v>
+      </c>
+      <c r="B877" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C877" t="s">
+        <v>946</v>
+      </c>
+      <c r="D877" t="s">
+        <v>877</v>
+      </c>
+      <c r="E877" t="s">
+        <v>878</v>
       </c>
     </row>
     <row r="878" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A878" t="s">
-        <v>1054</v>
+        <v>1047</v>
+      </c>
+      <c r="B878" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C878" t="s">
+        <v>946</v>
+      </c>
+      <c r="D878" t="s">
+        <v>877</v>
+      </c>
+      <c r="E878" t="s">
+        <v>878</v>
       </c>
     </row>
     <row r="879" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A879" t="s">
-        <v>1055</v>
+        <v>1047</v>
+      </c>
+      <c r="B879" t="s">
+        <v>1083</v>
+      </c>
+      <c r="C879" t="s">
+        <v>946</v>
+      </c>
+      <c r="D879" t="s">
+        <v>877</v>
+      </c>
+      <c r="E879" t="s">
+        <v>878</v>
       </c>
     </row>
     <row r="880" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A880" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B880" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C880" t="s">
+        <v>946</v>
+      </c>
+      <c r="D880" t="s">
+        <v>877</v>
+      </c>
+      <c r="E880" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="881" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A881" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B881" t="s">
+        <v>1085</v>
+      </c>
+      <c r="C881" t="s">
+        <v>946</v>
+      </c>
+      <c r="D881" t="s">
+        <v>877</v>
+      </c>
+      <c r="E881" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="882" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A882" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B882" t="s">
+        <v>1086</v>
+      </c>
+      <c r="C882" t="s">
+        <v>946</v>
+      </c>
+      <c r="D882" t="s">
+        <v>877</v>
+      </c>
+      <c r="E882" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="883" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A883" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B883" t="s">
+        <v>1087</v>
+      </c>
+      <c r="C883" t="s">
+        <v>946</v>
+      </c>
+      <c r="D883" t="s">
+        <v>877</v>
+      </c>
+      <c r="E883" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="884" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A884" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B884" s="3">
+        <v>1992</v>
+      </c>
+      <c r="C884" t="s">
+        <v>946</v>
+      </c>
+      <c r="D884" t="s">
+        <v>877</v>
+      </c>
+      <c r="E884" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="885" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A885" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B885" t="s">
+        <v>1088</v>
+      </c>
+      <c r="C885" t="s">
+        <v>946</v>
+      </c>
+      <c r="D885" t="s">
+        <v>877</v>
+      </c>
+      <c r="E885" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="886" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A886" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B886" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C886" t="s">
+        <v>946</v>
+      </c>
+      <c r="D886" t="s">
+        <v>877</v>
+      </c>
+      <c r="E886" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="887" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A887" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B887" t="s">
+        <v>1090</v>
+      </c>
+      <c r="C887" t="s">
+        <v>876</v>
+      </c>
+      <c r="D887" t="s">
+        <v>877</v>
+      </c>
+      <c r="E887" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="888" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A888" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B888" t="s">
+        <v>1091</v>
+      </c>
+      <c r="C888" t="s">
+        <v>876</v>
+      </c>
+      <c r="D888" t="s">
+        <v>877</v>
+      </c>
+      <c r="E888" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="889" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A889" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B889" t="s">
+        <v>1092</v>
+      </c>
+      <c r="C889" t="s">
+        <v>876</v>
+      </c>
+      <c r="D889" t="s">
+        <v>877</v>
+      </c>
+      <c r="E889" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="890" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A890" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B890" t="s">
+        <v>1093</v>
+      </c>
+      <c r="C890" t="s">
+        <v>876</v>
+      </c>
+      <c r="D890" t="s">
+        <v>877</v>
+      </c>
+      <c r="E890" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="891" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A891" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B891" t="s">
+        <v>1094</v>
+      </c>
+      <c r="C891" t="s">
+        <v>876</v>
+      </c>
+      <c r="D891" t="s">
+        <v>877</v>
+      </c>
+      <c r="E891" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="892" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A892" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B892" t="s">
+        <v>1095</v>
+      </c>
+      <c r="C892" t="s">
+        <v>876</v>
+      </c>
+      <c r="D892" t="s">
+        <v>877</v>
+      </c>
+      <c r="E892" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="893" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A893" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B893" t="s">
+        <v>1089</v>
+      </c>
+      <c r="C893" t="s">
+        <v>876</v>
+      </c>
+      <c r="D893" t="s">
+        <v>877</v>
+      </c>
+      <c r="E893" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="894" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A894" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B894" t="s">
+        <v>1096</v>
+      </c>
+      <c r="C894" t="s">
+        <v>876</v>
+      </c>
+      <c r="D894" t="s">
+        <v>877</v>
+      </c>
+      <c r="E894" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="895" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A895" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B895" t="s">
+        <v>1097</v>
+      </c>
+      <c r="C895" t="s">
+        <v>876</v>
+      </c>
+      <c r="D895" t="s">
+        <v>877</v>
+      </c>
+      <c r="E895" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="896" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A896" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B896" t="s">
+        <v>1098</v>
+      </c>
+      <c r="C896" t="s">
+        <v>876</v>
+      </c>
+      <c r="D896" t="s">
+        <v>877</v>
+      </c>
+      <c r="E896" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="897" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A897" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B897" t="s">
+        <v>1100</v>
+      </c>
+      <c r="C897" t="s">
+        <v>968</v>
+      </c>
+      <c r="D897" t="s">
+        <v>877</v>
+      </c>
+      <c r="E897" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="898" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A898" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B898" t="s">
+        <v>1101</v>
+      </c>
+      <c r="C898" t="s">
+        <v>968</v>
+      </c>
+      <c r="D898" t="s">
+        <v>877</v>
+      </c>
+      <c r="E898" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="899" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A899" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B899" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C899" t="s">
+        <v>968</v>
+      </c>
+      <c r="D899" t="s">
+        <v>877</v>
+      </c>
+      <c r="E899" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="900" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A900" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B900" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C900" t="s">
+        <v>968</v>
+      </c>
+      <c r="D900" t="s">
+        <v>877</v>
+      </c>
+      <c r="E900" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="901" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A901" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B901" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C901" t="s">
+        <v>968</v>
+      </c>
+      <c r="D901" t="s">
+        <v>877</v>
+      </c>
+      <c r="E901" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="902" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A902" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B902" t="s">
+        <v>1104</v>
+      </c>
+      <c r="C902" t="s">
+        <v>876</v>
+      </c>
+      <c r="D902" t="s">
+        <v>877</v>
+      </c>
+      <c r="E902" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="903" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A903" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B903" t="s">
+        <v>1105</v>
+      </c>
+      <c r="C903" t="s">
+        <v>876</v>
+      </c>
+      <c r="D903" t="s">
+        <v>877</v>
+      </c>
+      <c r="E903" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="904" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A904" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B904" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C904" t="s">
+        <v>876</v>
+      </c>
+      <c r="D904" t="s">
+        <v>877</v>
+      </c>
+      <c r="E904" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="905" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A905" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B905" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C905" t="s">
+        <v>876</v>
+      </c>
+      <c r="D905" t="s">
+        <v>877</v>
+      </c>
+      <c r="E905" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="906" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A906" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B906" t="s">
+        <v>1108</v>
+      </c>
+      <c r="C906" t="s">
+        <v>876</v>
+      </c>
+      <c r="D906" t="s">
+        <v>877</v>
+      </c>
+      <c r="E906" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="907" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A907" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B907" t="s">
+        <v>1103</v>
+      </c>
+      <c r="C907" t="s">
+        <v>876</v>
+      </c>
+      <c r="D907" t="s">
+        <v>877</v>
+      </c>
+      <c r="E907" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="908" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A908" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B908" t="s">
+        <v>1110</v>
+      </c>
+      <c r="C908" t="s">
+        <v>968</v>
+      </c>
+      <c r="D908" t="s">
+        <v>877</v>
+      </c>
+      <c r="E908" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="909" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A909" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B909" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C909" t="s">
+        <v>968</v>
+      </c>
+      <c r="D909" t="s">
+        <v>877</v>
+      </c>
+      <c r="E909" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="910" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A910" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B910" t="s">
+        <v>1112</v>
+      </c>
+      <c r="C910" t="s">
+        <v>968</v>
+      </c>
+      <c r="D910" t="s">
+        <v>877</v>
+      </c>
+      <c r="E910" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="911" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A911" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B911" t="s">
+        <v>1113</v>
+      </c>
+      <c r="C911" t="s">
+        <v>968</v>
+      </c>
+      <c r="D911" t="s">
+        <v>877</v>
+      </c>
+      <c r="E911" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="912" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A912" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B912" t="s">
+        <v>1114</v>
+      </c>
+      <c r="C912" t="s">
+        <v>968</v>
+      </c>
+      <c r="D912" t="s">
+        <v>877</v>
+      </c>
+      <c r="E912" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="913" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A913" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B913" t="s">
+        <v>1109</v>
+      </c>
+      <c r="C913" t="s">
+        <v>968</v>
+      </c>
+      <c r="D913" t="s">
+        <v>877</v>
+      </c>
+      <c r="E913" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="914" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A914" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B914" t="s">
+        <v>1115</v>
+      </c>
+      <c r="C914" t="s">
+        <v>876</v>
+      </c>
+      <c r="D914" t="s">
+        <v>877</v>
+      </c>
+      <c r="E914" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="915" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A915" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B915" s="3">
+        <v>90059</v>
+      </c>
+      <c r="C915" t="s">
+        <v>876</v>
+      </c>
+      <c r="D915" t="s">
+        <v>877</v>
+      </c>
+      <c r="E915" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="916" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A916" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B916" t="s">
+        <v>1116</v>
+      </c>
+      <c r="C916" t="s">
+        <v>876</v>
+      </c>
+      <c r="D916" t="s">
+        <v>877</v>
+      </c>
+      <c r="E916" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="917" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A917" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B917" t="s">
+        <v>1118</v>
+      </c>
+      <c r="C917" t="s">
+        <v>977</v>
+      </c>
+      <c r="D917" t="s">
+        <v>877</v>
+      </c>
+      <c r="E917" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="918" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A918" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B918" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C918" t="s">
+        <v>977</v>
+      </c>
+      <c r="D918" t="s">
+        <v>877</v>
+      </c>
+      <c r="E918" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="919" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A919" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B919" t="s">
+        <v>1120</v>
+      </c>
+      <c r="C919" t="s">
+        <v>977</v>
+      </c>
+      <c r="D919" t="s">
+        <v>877</v>
+      </c>
+      <c r="E919" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="920" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A920" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B920" t="s">
+        <v>1121</v>
+      </c>
+      <c r="C920" t="s">
+        <v>977</v>
+      </c>
+      <c r="D920" t="s">
+        <v>877</v>
+      </c>
+      <c r="E920" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="921" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A921" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B921" t="s">
+        <v>1122</v>
+      </c>
+      <c r="C921" t="s">
+        <v>977</v>
+      </c>
+      <c r="D921" t="s">
+        <v>877</v>
+      </c>
+      <c r="E921" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="922" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A922" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B922" t="s">
+        <v>1123</v>
+      </c>
+      <c r="C922" t="s">
+        <v>977</v>
+      </c>
+      <c r="D922" t="s">
+        <v>877</v>
+      </c>
+      <c r="E922" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="923" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A923" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B923" t="s">
+        <v>1124</v>
+      </c>
+      <c r="C923" t="s">
+        <v>977</v>
+      </c>
+      <c r="D923" t="s">
+        <v>877</v>
+      </c>
+      <c r="E923" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="924" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A924" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B924" t="s">
+        <v>1125</v>
+      </c>
+      <c r="C924" t="s">
+        <v>977</v>
+      </c>
+      <c r="D924" t="s">
+        <v>877</v>
+      </c>
+      <c r="E924" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="925" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A925" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B925" t="s">
+        <v>1126</v>
+      </c>
+      <c r="C925" t="s">
+        <v>977</v>
+      </c>
+      <c r="D925" t="s">
+        <v>877</v>
+      </c>
+      <c r="E925" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="926" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A926" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B926" t="s">
+        <v>1127</v>
+      </c>
+      <c r="C926" t="s">
+        <v>977</v>
+      </c>
+      <c r="D926" t="s">
+        <v>877</v>
+      </c>
+      <c r="E926" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="927" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A927" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B927" t="s">
+        <v>1117</v>
+      </c>
+      <c r="C927" t="s">
+        <v>977</v>
+      </c>
+      <c r="D927" t="s">
+        <v>877</v>
+      </c>
+      <c r="E927" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="928" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A928" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B928" t="s">
+        <v>1129</v>
+      </c>
+      <c r="C928" t="s">
+        <v>946</v>
+      </c>
+      <c r="D928" t="s">
+        <v>877</v>
+      </c>
+      <c r="E928" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="929" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A929" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B929" t="s">
+        <v>1128</v>
+      </c>
+      <c r="C929" t="s">
+        <v>946</v>
+      </c>
+      <c r="D929" t="s">
+        <v>877</v>
+      </c>
+      <c r="E929" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="930" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A930" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B930" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C930" t="s">
+        <v>946</v>
+      </c>
+      <c r="D930" t="s">
+        <v>877</v>
+      </c>
+      <c r="E930" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="931" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A931" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B931" t="s">
+        <v>1132</v>
+      </c>
+      <c r="C931" t="s">
+        <v>946</v>
+      </c>
+      <c r="D931" t="s">
+        <v>877</v>
+      </c>
+      <c r="E931" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="932" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A932" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B932" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C932" t="s">
+        <v>946</v>
+      </c>
+      <c r="D932" t="s">
+        <v>877</v>
+      </c>
+      <c r="E932" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="933" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A933" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B933" t="s">
+        <v>1134</v>
+      </c>
+      <c r="C933" t="s">
+        <v>946</v>
+      </c>
+      <c r="D933" t="s">
+        <v>877</v>
+      </c>
+      <c r="E933" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="934" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A934" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B934" t="s">
+        <v>1135</v>
+      </c>
+      <c r="C934" t="s">
+        <v>946</v>
+      </c>
+      <c r="D934" t="s">
+        <v>877</v>
+      </c>
+      <c r="E934" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="935" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A935" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B935" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C935" t="s">
+        <v>946</v>
+      </c>
+      <c r="D935" t="s">
+        <v>877</v>
+      </c>
+      <c r="E935" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="936" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A936" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B936" t="s">
+        <v>1137</v>
+      </c>
+      <c r="C936" t="s">
+        <v>946</v>
+      </c>
+      <c r="D936" t="s">
+        <v>877</v>
+      </c>
+      <c r="E936" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="937" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A937" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B937" t="s">
+        <v>1138</v>
+      </c>
+      <c r="C937" t="s">
+        <v>946</v>
+      </c>
+      <c r="D937" t="s">
+        <v>877</v>
+      </c>
+      <c r="E937" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="938" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A938" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B938" t="s">
+        <v>1130</v>
+      </c>
+      <c r="C938" t="s">
+        <v>946</v>
+      </c>
+      <c r="D938" t="s">
+        <v>877</v>
+      </c>
+      <c r="E938" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="939" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A939" t="s">
         <v>1056</v>
       </c>
-    </row>
-    <row r="881" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A881" t="s">
-        <v>1057</v>
+      <c r="B939" t="s">
+        <v>1140</v>
+      </c>
+      <c r="C939" t="s">
+        <v>876</v>
+      </c>
+      <c r="D939" t="s">
+        <v>877</v>
+      </c>
+      <c r="E939" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="940" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A940" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B940" t="s">
+        <v>1141</v>
+      </c>
+      <c r="C940" t="s">
+        <v>876</v>
+      </c>
+      <c r="D940" t="s">
+        <v>877</v>
+      </c>
+      <c r="E940" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="941" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A941" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B941" t="s">
+        <v>1142</v>
+      </c>
+      <c r="C941" t="s">
+        <v>876</v>
+      </c>
+      <c r="D941" t="s">
+        <v>877</v>
+      </c>
+      <c r="E941" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="942" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A942" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B942" t="s">
+        <v>1143</v>
+      </c>
+      <c r="C942" t="s">
+        <v>876</v>
+      </c>
+      <c r="D942" t="s">
+        <v>877</v>
+      </c>
+      <c r="E942" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="943" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A943" t="s">
+        <v>1056</v>
+      </c>
+      <c r="B943" t="s">
+        <v>1139</v>
+      </c>
+      <c r="C943" t="s">
+        <v>876</v>
+      </c>
+      <c r="D943" t="s">
+        <v>877</v>
+      </c>
+      <c r="E943" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="944" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A944" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B944" t="s">
+        <v>1145</v>
+      </c>
+      <c r="C944" t="s">
+        <v>350</v>
+      </c>
+      <c r="D944" t="s">
+        <v>340</v>
+      </c>
+      <c r="E944" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="945" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A945" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B945" t="s">
+        <v>1146</v>
+      </c>
+      <c r="C945" t="s">
+        <v>350</v>
+      </c>
+      <c r="D945" t="s">
+        <v>340</v>
+      </c>
+      <c r="E945" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="946" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A946" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B946" t="s">
+        <v>1147</v>
+      </c>
+      <c r="C946" t="s">
+        <v>350</v>
+      </c>
+      <c r="D946" t="s">
+        <v>340</v>
+      </c>
+      <c r="E946" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="947" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A947" t="s">
+        <v>1058</v>
+      </c>
+      <c r="B947" t="s">
+        <v>1144</v>
+      </c>
+      <c r="C947" t="s">
+        <v>350</v>
+      </c>
+      <c r="D947" t="s">
+        <v>340</v>
+      </c>
+      <c r="E947" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="948" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A948" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B948" t="s">
+        <v>1149</v>
+      </c>
+      <c r="C948" t="s">
+        <v>350</v>
+      </c>
+      <c r="D948" t="s">
+        <v>340</v>
+      </c>
+      <c r="E948" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="949" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A949" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B949" t="s">
+        <v>1150</v>
+      </c>
+      <c r="C949" t="s">
+        <v>350</v>
+      </c>
+      <c r="D949" t="s">
+        <v>340</v>
+      </c>
+      <c r="E949" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="950" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A950" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B950" t="s">
+        <v>1151</v>
+      </c>
+      <c r="C950" t="s">
+        <v>350</v>
+      </c>
+      <c r="D950" t="s">
+        <v>340</v>
+      </c>
+      <c r="E950" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="951" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A951" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B951" t="s">
+        <v>1152</v>
+      </c>
+      <c r="C951" t="s">
+        <v>350</v>
+      </c>
+      <c r="D951" t="s">
+        <v>340</v>
+      </c>
+      <c r="E951" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="952" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A952" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B952" t="s">
+        <v>1153</v>
+      </c>
+      <c r="C952" t="s">
+        <v>350</v>
+      </c>
+      <c r="D952" t="s">
+        <v>340</v>
+      </c>
+      <c r="E952" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="953" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A953" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B953" t="s">
+        <v>1154</v>
+      </c>
+      <c r="C953" t="s">
+        <v>350</v>
+      </c>
+      <c r="D953" t="s">
+        <v>340</v>
+      </c>
+      <c r="E953" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="954" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A954" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B954" t="s">
+        <v>1155</v>
+      </c>
+      <c r="C954" t="s">
+        <v>350</v>
+      </c>
+      <c r="D954" t="s">
+        <v>340</v>
+      </c>
+      <c r="E954" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="955" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A955" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B955" t="s">
+        <v>1148</v>
+      </c>
+      <c r="C955" t="s">
+        <v>350</v>
+      </c>
+      <c r="D955" t="s">
+        <v>340</v>
+      </c>
+      <c r="E955" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="956" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A956" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B956" t="s">
+        <v>1156</v>
+      </c>
+      <c r="C956" t="s">
+        <v>664</v>
+      </c>
+      <c r="D956" t="s">
+        <v>665</v>
+      </c>
+      <c r="E956" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="957" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A957" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B957" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C957" t="s">
+        <v>664</v>
+      </c>
+      <c r="D957" t="s">
+        <v>665</v>
+      </c>
+      <c r="E957" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="958" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A958" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B958" t="s">
+        <v>1158</v>
+      </c>
+      <c r="C958" t="s">
+        <v>664</v>
+      </c>
+      <c r="D958" t="s">
+        <v>665</v>
+      </c>
+      <c r="E958" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="959" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A959" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B959" t="s">
+        <v>1159</v>
+      </c>
+      <c r="C959" t="s">
+        <v>664</v>
+      </c>
+      <c r="D959" t="s">
+        <v>665</v>
+      </c>
+      <c r="E959" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="960" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A960" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B960" t="s">
+        <v>1160</v>
+      </c>
+      <c r="C960" t="s">
+        <v>664</v>
+      </c>
+      <c r="D960" t="s">
+        <v>665</v>
+      </c>
+      <c r="E960" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="961" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A961" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B961" t="s">
+        <v>1161</v>
+      </c>
+      <c r="C961" t="s">
+        <v>263</v>
+      </c>
+      <c r="D961" t="s">
+        <v>264</v>
+      </c>
+      <c r="E961" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="962" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A962" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B962" t="s">
+        <v>1162</v>
+      </c>
+      <c r="C962" t="s">
+        <v>263</v>
+      </c>
+      <c r="D962" t="s">
+        <v>264</v>
+      </c>
+      <c r="E962" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="963" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A963" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B963" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C963" t="s">
+        <v>263</v>
+      </c>
+      <c r="D963" t="s">
+        <v>264</v>
+      </c>
+      <c r="E963" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="964" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A964" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B964" t="s">
+        <v>1164</v>
+      </c>
+      <c r="C964" t="s">
+        <v>263</v>
+      </c>
+      <c r="D964" t="s">
+        <v>264</v>
+      </c>
+      <c r="E964" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="965" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A965" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B965" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C965" t="s">
+        <v>263</v>
+      </c>
+      <c r="D965" t="s">
+        <v>264</v>
+      </c>
+      <c r="E965" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="966" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A966" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B966" t="s">
+        <v>1166</v>
+      </c>
+      <c r="C966" t="s">
+        <v>263</v>
+      </c>
+      <c r="D966" t="s">
+        <v>264</v>
+      </c>
+      <c r="E966" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="967" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A967" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B967" t="s">
+        <v>1167</v>
+      </c>
+      <c r="C967" t="s">
+        <v>263</v>
+      </c>
+      <c r="D967" t="s">
+        <v>264</v>
+      </c>
+      <c r="E967" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="968" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A968" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B968" t="s">
+        <v>1168</v>
+      </c>
+      <c r="C968" t="s">
+        <v>263</v>
+      </c>
+      <c r="D968" t="s">
+        <v>264</v>
+      </c>
+      <c r="E968" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="969" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A969" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B969" t="s">
+        <v>1169</v>
+      </c>
+      <c r="C969" t="s">
+        <v>263</v>
+      </c>
+      <c r="D969" t="s">
+        <v>264</v>
+      </c>
+      <c r="E969" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="970" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A970" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B970" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C970" t="s">
+        <v>263</v>
+      </c>
+      <c r="D970" t="s">
+        <v>264</v>
+      </c>
+      <c r="E970" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="971" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A971" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B971" t="s">
+        <v>1171</v>
+      </c>
+      <c r="C971" t="s">
+        <v>263</v>
+      </c>
+      <c r="D971" t="s">
+        <v>264</v>
+      </c>
+      <c r="E971" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="972" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A972" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B972" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C972" t="s">
+        <v>263</v>
+      </c>
+      <c r="D972" t="s">
+        <v>264</v>
+      </c>
+      <c r="E972" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="973" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A973" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B973" t="s">
+        <v>1173</v>
+      </c>
+      <c r="C973" t="s">
+        <v>263</v>
+      </c>
+      <c r="D973" t="s">
+        <v>264</v>
+      </c>
+      <c r="E973" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="974" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A974" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B974" t="s">
+        <v>1174</v>
+      </c>
+      <c r="C974" t="s">
+        <v>263</v>
+      </c>
+      <c r="D974" t="s">
+        <v>264</v>
+      </c>
+      <c r="E974" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="975" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A975" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B975" t="s">
+        <v>1175</v>
+      </c>
+      <c r="C975" t="s">
+        <v>263</v>
+      </c>
+      <c r="D975" t="s">
+        <v>264</v>
+      </c>
+      <c r="E975" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="976" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A976" t="s">
+        <v>1061</v>
+      </c>
+      <c r="B976" t="s">
+        <v>1176</v>
+      </c>
+      <c r="C976" t="s">
+        <v>876</v>
+      </c>
+      <c r="D976" t="s">
+        <v>877</v>
+      </c>
+      <c r="E976" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="977" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A977" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B977" t="s">
+        <v>1179</v>
+      </c>
+      <c r="C977" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D977" t="s">
+        <v>877</v>
+      </c>
+      <c r="E977" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="978" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A978" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B978" t="s">
+        <v>1180</v>
+      </c>
+      <c r="C978" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D978" t="s">
+        <v>877</v>
+      </c>
+      <c r="E978" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="979" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A979" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B979" t="s">
+        <v>1181</v>
+      </c>
+      <c r="C979" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D979" t="s">
+        <v>877</v>
+      </c>
+      <c r="E979" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="980" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A980" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B980" t="s">
+        <v>1182</v>
+      </c>
+      <c r="C980" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D980" t="s">
+        <v>877</v>
+      </c>
+      <c r="E980" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="981" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A981" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B981" t="s">
+        <v>1183</v>
+      </c>
+      <c r="C981" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D981" t="s">
+        <v>877</v>
+      </c>
+      <c r="E981" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="982" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A982" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B982" t="s">
+        <v>1184</v>
+      </c>
+      <c r="C982" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D982" t="s">
+        <v>877</v>
+      </c>
+      <c r="E982" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="983" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A983" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B983" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C983" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D983" t="s">
+        <v>877</v>
+      </c>
+      <c r="E983" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="984" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A984" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B984" t="s">
+        <v>1186</v>
+      </c>
+      <c r="C984" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D984" t="s">
+        <v>877</v>
+      </c>
+      <c r="E984" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="985" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A985" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B985" t="s">
+        <v>1187</v>
+      </c>
+      <c r="C985" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D985" t="s">
+        <v>877</v>
+      </c>
+      <c r="E985" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="986" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A986" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B986" t="s">
+        <v>1188</v>
+      </c>
+      <c r="C986" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D986" t="s">
+        <v>877</v>
+      </c>
+      <c r="E986" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="987" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A987" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B987" t="s">
+        <v>1189</v>
+      </c>
+      <c r="C987" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D987" t="s">
+        <v>877</v>
+      </c>
+      <c r="E987" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="988" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A988" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B988" t="s">
+        <v>1190</v>
+      </c>
+      <c r="C988" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D988" t="s">
+        <v>877</v>
+      </c>
+      <c r="E988" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="989" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A989" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B989" t="s">
+        <v>1191</v>
+      </c>
+      <c r="C989" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D989" t="s">
+        <v>877</v>
+      </c>
+      <c r="E989" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="990" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A990" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B990" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C990" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D990" t="s">
+        <v>877</v>
+      </c>
+      <c r="E990" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="991" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A991" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B991" t="s">
+        <v>1193</v>
+      </c>
+      <c r="C991" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D991" t="s">
+        <v>877</v>
+      </c>
+      <c r="E991" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="992" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A992" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B992" t="s">
+        <v>1194</v>
+      </c>
+      <c r="C992" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D992" t="s">
+        <v>877</v>
+      </c>
+      <c r="E992" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="993" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A993" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B993" t="s">
+        <v>1195</v>
+      </c>
+      <c r="C993" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D993" t="s">
+        <v>877</v>
+      </c>
+      <c r="E993" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="994" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A994" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B994" t="s">
+        <v>1178</v>
+      </c>
+      <c r="C994" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D994" t="s">
+        <v>877</v>
+      </c>
+      <c r="E994" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="995" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A995" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B995" t="s">
+        <v>1196</v>
+      </c>
+      <c r="C995" t="s">
+        <v>263</v>
+      </c>
+      <c r="D995" t="s">
+        <v>264</v>
+      </c>
+      <c r="E995" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="996" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A996" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B996" t="s">
+        <v>1197</v>
+      </c>
+      <c r="C996" t="s">
+        <v>263</v>
+      </c>
+      <c r="D996" t="s">
+        <v>264</v>
+      </c>
+      <c r="E996" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="997" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A997" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B997" t="s">
+        <v>1198</v>
+      </c>
+      <c r="C997" t="s">
+        <v>263</v>
+      </c>
+      <c r="D997" t="s">
+        <v>264</v>
+      </c>
+      <c r="E997" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="998" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A998" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B998" s="5" t="s">
+        <v>1199</v>
+      </c>
+      <c r="C998" t="s">
+        <v>263</v>
+      </c>
+      <c r="D998" t="s">
+        <v>264</v>
+      </c>
+      <c r="E998" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="999" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A999" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B999" t="s">
+        <v>1200</v>
+      </c>
+      <c r="C999" t="s">
+        <v>263</v>
+      </c>
+      <c r="D999" t="s">
+        <v>264</v>
+      </c>
+      <c r="E999" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1000" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B1000" t="s">
+        <v>1201</v>
+      </c>
+      <c r="C1000" t="s">
+        <v>263</v>
+      </c>
+      <c r="D1000" t="s">
+        <v>264</v>
+      </c>
+      <c r="E1000" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="1001" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1001" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B1001" t="s">
+        <v>1202</v>
+      </c>
+      <c r="C1001" t="s">
+        <v>263</v>
+      </c>
+      <c r="D1001" t="s">
+        <v>264</v>
+      </c>
+      <c r="E1001" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="1002" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1002" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B1002" t="s">
+        <v>1203</v>
+      </c>
+      <c r="C1002" t="s">
+        <v>270</v>
+      </c>
+      <c r="D1002" t="s">
+        <v>271</v>
+      </c>
+      <c r="E1002" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1003" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B1003" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C1003" t="s">
+        <v>270</v>
+      </c>
+      <c r="D1003" t="s">
+        <v>271</v>
+      </c>
+      <c r="E1003" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1004" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B1004" t="s">
+        <v>1205</v>
+      </c>
+      <c r="C1004" t="s">
+        <v>270</v>
+      </c>
+      <c r="D1004" t="s">
+        <v>271</v>
+      </c>
+      <c r="E1004" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1005" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B1005" t="s">
+        <v>1208</v>
+      </c>
+      <c r="C1005" t="s">
+        <v>977</v>
+      </c>
+      <c r="D1005" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1005" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1006" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B1006" t="s">
+        <v>1209</v>
+      </c>
+      <c r="C1006" t="s">
+        <v>977</v>
+      </c>
+      <c r="D1006" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1006" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1007" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B1007" t="s">
+        <v>1210</v>
+      </c>
+      <c r="C1007" t="s">
+        <v>977</v>
+      </c>
+      <c r="D1007" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1007" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1008" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B1008" t="s">
+        <v>1211</v>
+      </c>
+      <c r="C1008" t="s">
+        <v>977</v>
+      </c>
+      <c r="D1008" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1008" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1009" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B1009" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C1009" t="s">
+        <v>977</v>
+      </c>
+      <c r="D1009" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1009" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1010" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B1010" t="s">
+        <v>1213</v>
+      </c>
+      <c r="C1010" t="s">
+        <v>977</v>
+      </c>
+      <c r="D1010" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1010" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1011" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B1011" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C1011" t="s">
+        <v>977</v>
+      </c>
+      <c r="D1011" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1011" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1012" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1012" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B1012" t="s">
+        <v>1215</v>
+      </c>
+      <c r="C1012" t="s">
+        <v>977</v>
+      </c>
+      <c r="D1012" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1012" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1013" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B1013" t="s">
+        <v>1216</v>
+      </c>
+      <c r="C1013" t="s">
+        <v>977</v>
+      </c>
+      <c r="D1013" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1013" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1014" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B1014" t="s">
+        <v>1217</v>
+      </c>
+      <c r="C1014" t="s">
+        <v>977</v>
+      </c>
+      <c r="D1014" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1014" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1015" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B1015" t="s">
+        <v>1207</v>
+      </c>
+      <c r="C1015" t="s">
+        <v>977</v>
+      </c>
+      <c r="D1015" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1015" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1016" t="s">
+        <v>1067</v>
+      </c>
+      <c r="B1016" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C1016" t="s">
+        <v>516</v>
+      </c>
+      <c r="D1016" t="s">
+        <v>340</v>
+      </c>
+      <c r="E1016" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1017" t="s">
+        <v>1067</v>
+      </c>
+      <c r="B1017" t="s">
+        <v>1221</v>
+      </c>
+      <c r="C1017" t="s">
+        <v>516</v>
+      </c>
+      <c r="D1017" t="s">
+        <v>340</v>
+      </c>
+      <c r="E1017" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1018" t="s">
+        <v>1067</v>
+      </c>
+      <c r="B1018" t="s">
+        <v>1219</v>
+      </c>
+      <c r="C1018" t="s">
+        <v>516</v>
+      </c>
+      <c r="D1018" t="s">
+        <v>340</v>
+      </c>
+      <c r="E1018" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="1019" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1019" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B1019" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C1019" t="s">
+        <v>273</v>
+      </c>
+      <c r="D1019" t="s">
+        <v>272</v>
+      </c>
+      <c r="E1019" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="1020" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1020" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B1020" t="s">
+        <v>1223</v>
+      </c>
+      <c r="C1020" t="s">
+        <v>273</v>
+      </c>
+      <c r="D1020" t="s">
+        <v>272</v>
+      </c>
+      <c r="E1020" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="1021" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1021" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B1021" t="s">
+        <v>1224</v>
+      </c>
+      <c r="C1021" t="s">
+        <v>273</v>
+      </c>
+      <c r="D1021" t="s">
+        <v>272</v>
+      </c>
+      <c r="E1021" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="1022" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1022" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B1022" t="s">
+        <v>1225</v>
+      </c>
+      <c r="C1022" t="s">
+        <v>422</v>
+      </c>
+      <c r="D1022" t="s">
+        <v>340</v>
+      </c>
+      <c r="E1022" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="1023" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1023" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B1023" t="s">
+        <v>1226</v>
+      </c>
+      <c r="C1023" t="s">
+        <v>422</v>
+      </c>
+      <c r="D1023" t="s">
+        <v>340</v>
+      </c>
+      <c r="E1023" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="1024" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1024" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B1024" t="s">
+        <v>1227</v>
+      </c>
+      <c r="C1024" t="s">
+        <v>422</v>
+      </c>
+      <c r="D1024" t="s">
+        <v>340</v>
+      </c>
+      <c r="E1024" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="1025" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1025" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B1025" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C1025" t="s">
+        <v>422</v>
+      </c>
+      <c r="D1025" t="s">
+        <v>340</v>
+      </c>
+      <c r="E1025" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="1026" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1026" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B1026" t="s">
+        <v>1229</v>
+      </c>
+      <c r="C1026" t="s">
+        <v>422</v>
+      </c>
+      <c r="D1026" t="s">
+        <v>340</v>
+      </c>
+      <c r="E1026" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="1027" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1027" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B1027" t="s">
+        <v>1070</v>
+      </c>
+      <c r="C1027" t="s">
+        <v>876</v>
+      </c>
+      <c r="D1027" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1027" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1028" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1028" t="s">
+        <v>1233</v>
+      </c>
+      <c r="B1028" t="s">
+        <v>1230</v>
+      </c>
+      <c r="C1028" t="s">
+        <v>876</v>
+      </c>
+      <c r="D1028" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1028" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1029" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1029" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B1029" t="s">
+        <v>1231</v>
+      </c>
+      <c r="C1029" t="s">
+        <v>876</v>
+      </c>
+      <c r="D1029" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1029" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1030" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1030" t="s">
+        <v>1235</v>
+      </c>
+      <c r="B1030" t="s">
+        <v>1232</v>
+      </c>
+      <c r="C1030" t="s">
+        <v>876</v>
+      </c>
+      <c r="D1030" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1030" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1031" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1031" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B1031" s="6" t="s">
+        <v>1237</v>
+      </c>
+      <c r="C1031" t="s">
+        <v>339</v>
+      </c>
+      <c r="D1031" t="s">
+        <v>340</v>
+      </c>
+      <c r="E1031" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="1032" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1032" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B1032" s="6" t="s">
+        <v>1238</v>
+      </c>
+      <c r="C1032" t="s">
+        <v>339</v>
+      </c>
+      <c r="D1032" t="s">
+        <v>340</v>
+      </c>
+      <c r="E1032" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="1033" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1033" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B1033" s="6" t="s">
+        <v>1239</v>
+      </c>
+      <c r="C1033" t="s">
+        <v>339</v>
+      </c>
+      <c r="D1033" t="s">
+        <v>340</v>
+      </c>
+      <c r="E1033" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="1034" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1034" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B1034" s="6" t="s">
+        <v>1240</v>
+      </c>
+      <c r="C1034" t="s">
+        <v>339</v>
+      </c>
+      <c r="D1034" t="s">
+        <v>340</v>
+      </c>
+      <c r="E1034" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="1035" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1035" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B1035" s="6" t="s">
+        <v>1241</v>
+      </c>
+      <c r="C1035" t="s">
+        <v>339</v>
+      </c>
+      <c r="D1035" t="s">
+        <v>340</v>
+      </c>
+      <c r="E1035" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="1036" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1036" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B1036" s="6" t="s">
+        <v>1242</v>
+      </c>
+      <c r="C1036" t="s">
+        <v>339</v>
+      </c>
+      <c r="D1036" t="s">
+        <v>340</v>
+      </c>
+      <c r="E1036" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="1037" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1037" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B1037" s="6" t="s">
+        <v>1236</v>
+      </c>
+      <c r="C1037" t="s">
+        <v>339</v>
+      </c>
+      <c r="D1037" t="s">
+        <v>340</v>
+      </c>
+      <c r="E1037" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="1038" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1038" t="s">
+        <v>1243</v>
+      </c>
+      <c r="B1038" t="s">
+        <v>1246</v>
+      </c>
+      <c r="C1038" t="s">
+        <v>1244</v>
+      </c>
+      <c r="D1038" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1038" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1039" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1039" t="s">
+        <v>1243</v>
+      </c>
+      <c r="B1039" t="s">
+        <v>1247</v>
+      </c>
+      <c r="C1039" t="s">
+        <v>1244</v>
+      </c>
+      <c r="D1039" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1039" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1040" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1040" t="s">
+        <v>1243</v>
+      </c>
+      <c r="B1040" t="s">
+        <v>1244</v>
+      </c>
+      <c r="C1040" t="s">
+        <v>1244</v>
+      </c>
+      <c r="D1040" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1040" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1041" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1041" t="s">
+        <v>1243</v>
+      </c>
+      <c r="B1041" t="s">
+        <v>1245</v>
+      </c>
+      <c r="C1041" t="s">
+        <v>1244</v>
+      </c>
+      <c r="D1041" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1041" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1042" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1042" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B1042" t="s">
+        <v>1250</v>
+      </c>
+      <c r="C1042" t="s">
+        <v>876</v>
+      </c>
+      <c r="D1042" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1042" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1043" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1043" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B1043" t="s">
+        <v>1251</v>
+      </c>
+      <c r="C1043" t="s">
+        <v>876</v>
+      </c>
+      <c r="D1043" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1043" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1044" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1044" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B1044" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C1044" t="s">
+        <v>876</v>
+      </c>
+      <c r="D1044" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1044" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1045" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1045" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B1045" t="s">
+        <v>1253</v>
+      </c>
+      <c r="C1045" t="s">
+        <v>876</v>
+      </c>
+      <c r="D1045" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1045" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1046" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1046" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B1046" t="s">
+        <v>1254</v>
+      </c>
+      <c r="C1046" t="s">
+        <v>876</v>
+      </c>
+      <c r="D1046" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1046" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1047" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1047" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B1047" t="s">
+        <v>1255</v>
+      </c>
+      <c r="C1047" t="s">
+        <v>876</v>
+      </c>
+      <c r="D1047" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1047" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1048" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1048" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B1048" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C1048" t="s">
+        <v>876</v>
+      </c>
+      <c r="D1048" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1048" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1049" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1049" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B1049" t="s">
+        <v>1257</v>
+      </c>
+      <c r="C1049" t="s">
+        <v>876</v>
+      </c>
+      <c r="D1049" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1049" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1050" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1050" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B1050" t="s">
+        <v>1248</v>
+      </c>
+      <c r="C1050" t="s">
+        <v>876</v>
+      </c>
+      <c r="D1050" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1050" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1051" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1051" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B1051" t="s">
+        <v>1258</v>
+      </c>
+      <c r="C1051" t="s">
+        <v>876</v>
+      </c>
+      <c r="D1051" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1051" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1052" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1052" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B1052" t="s">
+        <v>1259</v>
+      </c>
+      <c r="C1052" t="s">
+        <v>876</v>
+      </c>
+      <c r="D1052" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1052" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1053" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1053" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B1053" t="s">
+        <v>1249</v>
+      </c>
+      <c r="C1053" t="s">
+        <v>876</v>
+      </c>
+      <c r="D1053" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1053" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1054" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1054" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B1054" t="s">
+        <v>1261</v>
+      </c>
+      <c r="C1054" t="s">
+        <v>876</v>
+      </c>
+      <c r="D1054" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1054" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1055" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1055" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B1055" t="s">
+        <v>1262</v>
+      </c>
+      <c r="C1055" t="s">
+        <v>876</v>
+      </c>
+      <c r="D1055" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1055" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1056" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1056" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B1056" t="s">
+        <v>1263</v>
+      </c>
+      <c r="C1056" t="s">
+        <v>876</v>
+      </c>
+      <c r="D1056" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1056" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1057" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1057" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B1057" t="s">
+        <v>1264</v>
+      </c>
+      <c r="C1057" t="s">
+        <v>876</v>
+      </c>
+      <c r="D1057" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1057" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1058" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1058" t="s">
+        <v>1206</v>
+      </c>
+      <c r="B1058" t="s">
+        <v>1265</v>
+      </c>
+      <c r="C1058" t="s">
+        <v>977</v>
+      </c>
+      <c r="D1058" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1058" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1059" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1059" t="s">
+        <v>1206</v>
+      </c>
+      <c r="B1059" t="s">
+        <v>1266</v>
+      </c>
+      <c r="C1059" t="s">
+        <v>977</v>
+      </c>
+      <c r="D1059" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1059" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1060" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1060" t="s">
+        <v>1206</v>
+      </c>
+      <c r="B1060" t="s">
+        <v>1267</v>
+      </c>
+      <c r="C1060" t="s">
+        <v>977</v>
+      </c>
+      <c r="D1060" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1060" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1061" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1061" t="s">
+        <v>1206</v>
+      </c>
+      <c r="B1061" t="s">
+        <v>1268</v>
+      </c>
+      <c r="C1061" t="s">
+        <v>977</v>
+      </c>
+      <c r="D1061" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1061" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1062" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1062" t="s">
+        <v>1206</v>
+      </c>
+      <c r="B1062" t="s">
+        <v>1269</v>
+      </c>
+      <c r="C1062" t="s">
+        <v>977</v>
+      </c>
+      <c r="D1062" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1062" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1063" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1063" t="s">
+        <v>1206</v>
+      </c>
+      <c r="B1063" t="s">
+        <v>1270</v>
+      </c>
+      <c r="C1063" t="s">
+        <v>977</v>
+      </c>
+      <c r="D1063" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1063" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1064" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1064" t="s">
+        <v>1218</v>
+      </c>
+      <c r="B1064" t="s">
+        <v>1218</v>
+      </c>
+      <c r="C1064" t="s">
+        <v>1271</v>
+      </c>
+      <c r="D1064" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1064" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1065" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1065" t="s">
+        <v>1218</v>
+      </c>
+      <c r="B1065" t="s">
+        <v>1273</v>
+      </c>
+      <c r="C1065" t="s">
+        <v>1271</v>
+      </c>
+      <c r="D1065" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1065" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1066" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1066" t="s">
+        <v>1218</v>
+      </c>
+      <c r="B1066" t="s">
+        <v>1274</v>
+      </c>
+      <c r="C1066" t="s">
+        <v>1271</v>
+      </c>
+      <c r="D1066" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1066" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1067" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1067" t="s">
+        <v>1218</v>
+      </c>
+      <c r="B1067" t="s">
+        <v>1275</v>
+      </c>
+      <c r="C1067" t="s">
+        <v>1271</v>
+      </c>
+      <c r="D1067" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1067" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1068" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1068" t="s">
+        <v>1218</v>
+      </c>
+      <c r="B1068" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1068" t="s">
+        <v>1271</v>
+      </c>
+      <c r="D1068" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1068" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1069" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1069" t="s">
+        <v>1218</v>
+      </c>
+      <c r="B1069" t="s">
+        <v>1277</v>
+      </c>
+      <c r="C1069" t="s">
+        <v>1271</v>
+      </c>
+      <c r="D1069" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1069" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1070" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1070" t="s">
+        <v>1218</v>
+      </c>
+      <c r="B1070" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1070" t="s">
+        <v>1271</v>
+      </c>
+      <c r="D1070" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1070" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1071" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1071" t="s">
+        <v>1218</v>
+      </c>
+      <c r="B1071" t="s">
+        <v>1278</v>
+      </c>
+      <c r="C1071" t="s">
+        <v>1271</v>
+      </c>
+      <c r="D1071" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1071" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1072" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1072" t="s">
+        <v>1218</v>
+      </c>
+      <c r="B1072" t="s">
+        <v>1279</v>
+      </c>
+      <c r="C1072" t="s">
+        <v>1271</v>
+      </c>
+      <c r="D1072" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1072" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="1073" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1073" t="s">
+        <v>1218</v>
+      </c>
+      <c r="B1073" t="s">
+        <v>1272</v>
+      </c>
+      <c r="C1073" t="s">
+        <v>1271</v>
+      </c>
+      <c r="D1073" t="s">
+        <v>877</v>
+      </c>
+      <c r="E1073" t="s">
+        <v>878</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more midwest and female artists to db.
</commit_message>
<xml_diff>
--- a/album_list.xlsx
+++ b/album_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP USER\Coding\Play\Rap_Lyrics\lyricsNLP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B6953F-A6CA-4EF6-8653-071F9056FE4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AEF1259-D2AD-4287-8E4C-1000DC10887C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-10005" windowWidth="29040" windowHeight="15720" xr2:uid="{4CD478C6-4722-4BC8-838A-CC153C60C18A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4CD478C6-4722-4BC8-838A-CC153C60C18A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5278" uniqueCount="1250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5492" uniqueCount="1300">
   <si>
     <t>Artist</t>
   </si>
@@ -3786,6 +3786,156 @@
   </si>
   <si>
     <t>Michael</t>
+  </si>
+  <si>
+    <t>Jadakiss</t>
+  </si>
+  <si>
+    <t>Ignatius</t>
+  </si>
+  <si>
+    <t>Kiss tha Game Goodbye</t>
+  </si>
+  <si>
+    <t>Kiss of Death</t>
+  </si>
+  <si>
+    <t>The Last Kiss</t>
+  </si>
+  <si>
+    <t>Top 5 Dead or Alive</t>
+  </si>
+  <si>
+    <t>Cordae</t>
+  </si>
+  <si>
+    <t>The Lost Boy</t>
+  </si>
+  <si>
+    <t>From a Birds Eye View</t>
+  </si>
+  <si>
+    <t>Broke With Expensive Taste</t>
+  </si>
+  <si>
+    <t>Azealia Banks</t>
+  </si>
+  <si>
+    <t>Icy Colors Change</t>
+  </si>
+  <si>
+    <t>Fantasea</t>
+  </si>
+  <si>
+    <t>Slay-Z</t>
+  </si>
+  <si>
+    <t>Yung Rapunxel PT. II</t>
+  </si>
+  <si>
+    <t>Danny Brown</t>
+  </si>
+  <si>
+    <t>The Hybrid</t>
+  </si>
+  <si>
+    <t>XXX</t>
+  </si>
+  <si>
+    <t>Old</t>
+  </si>
+  <si>
+    <t>Atrocity Exhibition</t>
+  </si>
+  <si>
+    <t>UKnowWhatImSayin</t>
+  </si>
+  <si>
+    <t>Detroit State of Mind</t>
+  </si>
+  <si>
+    <t>Detroit State of Mind 2</t>
+  </si>
+  <si>
+    <t>Detroit State of Mind 3</t>
+  </si>
+  <si>
+    <t>Detroit State of Mind 4</t>
+  </si>
+  <si>
+    <t>Hot Soup</t>
+  </si>
+  <si>
+    <t>It's a Art</t>
+  </si>
+  <si>
+    <t>Da Brat</t>
+  </si>
+  <si>
+    <t>Funkdafied</t>
+  </si>
+  <si>
+    <t>Anuthatantrum</t>
+  </si>
+  <si>
+    <t>Unrestricted</t>
+  </si>
+  <si>
+    <t>Limelite, Luv &amp; Niteclubz</t>
+  </si>
+  <si>
+    <t>Bow Wow</t>
+  </si>
+  <si>
+    <t>Vic Mensa</t>
+  </si>
+  <si>
+    <t>The Autobiography</t>
+  </si>
+  <si>
+    <t>Innanetape</t>
+  </si>
+  <si>
+    <t>Straight Up</t>
+  </si>
+  <si>
+    <t>The Manuscript</t>
+  </si>
+  <si>
+    <t>There's alot Going On</t>
+  </si>
+  <si>
+    <t>V Tape</t>
+  </si>
+  <si>
+    <t>I Tape</t>
+  </si>
+  <si>
+    <t>Vino Valentino</t>
+  </si>
+  <si>
+    <t>Hooligans</t>
+  </si>
+  <si>
+    <t>New Jack City II</t>
+  </si>
+  <si>
+    <t>Beware of Dog</t>
+  </si>
+  <si>
+    <t>Doggy Bag</t>
+  </si>
+  <si>
+    <t>Unleashed</t>
+  </si>
+  <si>
+    <t>Wanted</t>
+  </si>
+  <si>
+    <t>The Price of Fame</t>
+  </si>
+  <si>
+    <t>Columbus</t>
   </si>
 </sst>
 </file>
@@ -4187,10 +4337,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71A19CDE-E3DD-497E-8468-EF613F78BA90}">
-  <dimension ref="A1:E1058"/>
+  <dimension ref="A1:E1101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="G615" sqref="G615"/>
+    <sheetView tabSelected="1" topLeftCell="A1087" workbookViewId="0">
+      <selection activeCell="C1096" sqref="C1096:E1101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -22175,6 +22325,737 @@
       </c>
       <c r="E1058" t="s">
         <v>849</v>
+      </c>
+    </row>
+    <row r="1059" spans="1:5">
+      <c r="A1059" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B1059" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C1059" t="s">
+        <v>560</v>
+      </c>
+      <c r="D1059" t="s">
+        <v>329</v>
+      </c>
+      <c r="E1059" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="1060" spans="1:5">
+      <c r="A1060" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B1060" t="s">
+        <v>1253</v>
+      </c>
+      <c r="C1060" t="s">
+        <v>560</v>
+      </c>
+      <c r="D1060" t="s">
+        <v>329</v>
+      </c>
+      <c r="E1060" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="1061" spans="1:5">
+      <c r="A1061" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B1061" t="s">
+        <v>1254</v>
+      </c>
+      <c r="C1061" t="s">
+        <v>560</v>
+      </c>
+      <c r="D1061" t="s">
+        <v>329</v>
+      </c>
+      <c r="E1061" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="1062" spans="1:5">
+      <c r="A1062" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B1062" t="s">
+        <v>1255</v>
+      </c>
+      <c r="C1062" t="s">
+        <v>560</v>
+      </c>
+      <c r="D1062" t="s">
+        <v>329</v>
+      </c>
+      <c r="E1062" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="1063" spans="1:5">
+      <c r="A1063" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B1063" t="s">
+        <v>1251</v>
+      </c>
+      <c r="C1063" t="s">
+        <v>560</v>
+      </c>
+      <c r="D1063" t="s">
+        <v>329</v>
+      </c>
+      <c r="E1063" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="1064" spans="1:5">
+      <c r="A1064" t="s">
+        <v>1256</v>
+      </c>
+      <c r="B1064" t="s">
+        <v>1257</v>
+      </c>
+      <c r="C1064" t="s">
+        <v>267</v>
+      </c>
+      <c r="D1064" t="s">
+        <v>266</v>
+      </c>
+      <c r="E1064" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="1065" spans="1:5">
+      <c r="A1065" t="s">
+        <v>1256</v>
+      </c>
+      <c r="B1065" t="s">
+        <v>1258</v>
+      </c>
+      <c r="C1065" t="s">
+        <v>267</v>
+      </c>
+      <c r="D1065" t="s">
+        <v>266</v>
+      </c>
+      <c r="E1065" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="1066" spans="1:5">
+      <c r="A1066" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B1066" t="s">
+        <v>1259</v>
+      </c>
+      <c r="C1066" t="s">
+        <v>502</v>
+      </c>
+      <c r="D1066" t="s">
+        <v>329</v>
+      </c>
+      <c r="E1066" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="1067" spans="1:5">
+      <c r="A1067" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B1067" t="s">
+        <v>1261</v>
+      </c>
+      <c r="C1067" t="s">
+        <v>502</v>
+      </c>
+      <c r="D1067" t="s">
+        <v>329</v>
+      </c>
+      <c r="E1067" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="1068" spans="1:5">
+      <c r="A1068" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B1068" s="3">
+        <v>1991</v>
+      </c>
+      <c r="C1068" t="s">
+        <v>502</v>
+      </c>
+      <c r="D1068" t="s">
+        <v>329</v>
+      </c>
+      <c r="E1068" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="1069" spans="1:5">
+      <c r="A1069" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B1069" t="s">
+        <v>1262</v>
+      </c>
+      <c r="C1069" t="s">
+        <v>502</v>
+      </c>
+      <c r="D1069" t="s">
+        <v>329</v>
+      </c>
+      <c r="E1069" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="1070" spans="1:5">
+      <c r="A1070" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B1070" t="s">
+        <v>1263</v>
+      </c>
+      <c r="C1070" t="s">
+        <v>502</v>
+      </c>
+      <c r="D1070" t="s">
+        <v>329</v>
+      </c>
+      <c r="E1070" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="1071" spans="1:5">
+      <c r="A1071" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B1071" t="s">
+        <v>1264</v>
+      </c>
+      <c r="C1071" t="s">
+        <v>502</v>
+      </c>
+      <c r="D1071" t="s">
+        <v>329</v>
+      </c>
+      <c r="E1071" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="1072" spans="1:5">
+      <c r="A1072" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B1072" t="s">
+        <v>1266</v>
+      </c>
+      <c r="C1072" t="s">
+        <v>695</v>
+      </c>
+      <c r="D1072" t="s">
+        <v>696</v>
+      </c>
+      <c r="E1072" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="1073" spans="1:5">
+      <c r="A1073" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B1073" t="s">
+        <v>1267</v>
+      </c>
+      <c r="C1073" t="s">
+        <v>695</v>
+      </c>
+      <c r="D1073" t="s">
+        <v>696</v>
+      </c>
+      <c r="E1073" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="1074" spans="1:5">
+      <c r="A1074" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B1074" t="s">
+        <v>1268</v>
+      </c>
+      <c r="C1074" t="s">
+        <v>695</v>
+      </c>
+      <c r="D1074" t="s">
+        <v>696</v>
+      </c>
+      <c r="E1074" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="1075" spans="1:5">
+      <c r="A1075" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B1075" t="s">
+        <v>1269</v>
+      </c>
+      <c r="C1075" t="s">
+        <v>695</v>
+      </c>
+      <c r="D1075" t="s">
+        <v>696</v>
+      </c>
+      <c r="E1075" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="1076" spans="1:5">
+      <c r="A1076" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B1076" t="s">
+        <v>1270</v>
+      </c>
+      <c r="C1076" t="s">
+        <v>695</v>
+      </c>
+      <c r="D1076" t="s">
+        <v>696</v>
+      </c>
+      <c r="E1076" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="1077" spans="1:5">
+      <c r="A1077" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B1077" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C1077" t="s">
+        <v>695</v>
+      </c>
+      <c r="D1077" t="s">
+        <v>696</v>
+      </c>
+      <c r="E1077" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="1078" spans="1:5">
+      <c r="A1078" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B1078" t="s">
+        <v>1272</v>
+      </c>
+      <c r="C1078" t="s">
+        <v>695</v>
+      </c>
+      <c r="D1078" t="s">
+        <v>696</v>
+      </c>
+      <c r="E1078" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="1079" spans="1:5">
+      <c r="A1079" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B1079" t="s">
+        <v>1273</v>
+      </c>
+      <c r="C1079" t="s">
+        <v>695</v>
+      </c>
+      <c r="D1079" t="s">
+        <v>696</v>
+      </c>
+      <c r="E1079" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="1080" spans="1:5">
+      <c r="A1080" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B1080" t="s">
+        <v>1274</v>
+      </c>
+      <c r="C1080" t="s">
+        <v>695</v>
+      </c>
+      <c r="D1080" t="s">
+        <v>696</v>
+      </c>
+      <c r="E1080" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="1081" spans="1:5">
+      <c r="A1081" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B1081" t="s">
+        <v>1275</v>
+      </c>
+      <c r="C1081" t="s">
+        <v>695</v>
+      </c>
+      <c r="D1081" t="s">
+        <v>696</v>
+      </c>
+      <c r="E1081" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="1082" spans="1:5">
+      <c r="A1082" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B1082" t="s">
+        <v>1276</v>
+      </c>
+      <c r="C1082" t="s">
+        <v>695</v>
+      </c>
+      <c r="D1082" t="s">
+        <v>696</v>
+      </c>
+      <c r="E1082" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="1083" spans="1:5">
+      <c r="A1083" t="s">
+        <v>1277</v>
+      </c>
+      <c r="B1083" t="s">
+        <v>1278</v>
+      </c>
+      <c r="C1083" t="s">
+        <v>649</v>
+      </c>
+      <c r="D1083" t="s">
+        <v>650</v>
+      </c>
+      <c r="E1083" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="1084" spans="1:5">
+      <c r="A1084" t="s">
+        <v>1277</v>
+      </c>
+      <c r="B1084" t="s">
+        <v>1279</v>
+      </c>
+      <c r="C1084" t="s">
+        <v>649</v>
+      </c>
+      <c r="D1084" t="s">
+        <v>650</v>
+      </c>
+      <c r="E1084" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="1085" spans="1:5">
+      <c r="A1085" t="s">
+        <v>1277</v>
+      </c>
+      <c r="B1085" t="s">
+        <v>1280</v>
+      </c>
+      <c r="C1085" t="s">
+        <v>649</v>
+      </c>
+      <c r="D1085" t="s">
+        <v>650</v>
+      </c>
+      <c r="E1085" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="1086" spans="1:5">
+      <c r="A1086" t="s">
+        <v>1277</v>
+      </c>
+      <c r="B1086" t="s">
+        <v>1281</v>
+      </c>
+      <c r="C1086" t="s">
+        <v>649</v>
+      </c>
+      <c r="D1086" t="s">
+        <v>650</v>
+      </c>
+      <c r="E1086" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="1087" spans="1:5">
+      <c r="A1087" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B1087" t="s">
+        <v>1284</v>
+      </c>
+      <c r="C1087" t="s">
+        <v>649</v>
+      </c>
+      <c r="D1087" t="s">
+        <v>650</v>
+      </c>
+      <c r="E1087" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="1088" spans="1:5">
+      <c r="A1088" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B1088" t="s">
+        <v>1285</v>
+      </c>
+      <c r="C1088" t="s">
+        <v>649</v>
+      </c>
+      <c r="D1088" t="s">
+        <v>650</v>
+      </c>
+      <c r="E1088" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="1089" spans="1:5">
+      <c r="A1089" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B1089" t="s">
+        <v>1286</v>
+      </c>
+      <c r="C1089" t="s">
+        <v>649</v>
+      </c>
+      <c r="D1089" t="s">
+        <v>650</v>
+      </c>
+      <c r="E1089" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="1090" spans="1:5">
+      <c r="A1090" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B1090" t="s">
+        <v>1287</v>
+      </c>
+      <c r="C1090" t="s">
+        <v>649</v>
+      </c>
+      <c r="D1090" t="s">
+        <v>650</v>
+      </c>
+      <c r="E1090" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="1091" spans="1:5">
+      <c r="A1091" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B1091" t="s">
+        <v>1288</v>
+      </c>
+      <c r="C1091" t="s">
+        <v>649</v>
+      </c>
+      <c r="D1091" t="s">
+        <v>650</v>
+      </c>
+      <c r="E1091" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="1092" spans="1:5">
+      <c r="A1092" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B1092" t="s">
+        <v>1289</v>
+      </c>
+      <c r="C1092" t="s">
+        <v>649</v>
+      </c>
+      <c r="D1092" t="s">
+        <v>650</v>
+      </c>
+      <c r="E1092" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="1093" spans="1:5">
+      <c r="A1093" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B1093" t="s">
+        <v>1290</v>
+      </c>
+      <c r="C1093" t="s">
+        <v>649</v>
+      </c>
+      <c r="D1093" t="s">
+        <v>650</v>
+      </c>
+      <c r="E1093" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="1094" spans="1:5">
+      <c r="A1094" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B1094" t="s">
+        <v>1291</v>
+      </c>
+      <c r="C1094" t="s">
+        <v>649</v>
+      </c>
+      <c r="D1094" t="s">
+        <v>650</v>
+      </c>
+      <c r="E1094" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="1095" spans="1:5">
+      <c r="A1095" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B1095" t="s">
+        <v>1292</v>
+      </c>
+      <c r="C1095" t="s">
+        <v>649</v>
+      </c>
+      <c r="D1095" t="s">
+        <v>650</v>
+      </c>
+      <c r="E1095" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="1096" spans="1:5">
+      <c r="A1096" t="s">
+        <v>1282</v>
+      </c>
+      <c r="B1096" t="s">
+        <v>1294</v>
+      </c>
+      <c r="C1096" t="s">
+        <v>1299</v>
+      </c>
+      <c r="D1096" t="s">
+        <v>683</v>
+      </c>
+      <c r="E1096" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="1097" spans="1:5">
+      <c r="A1097" t="s">
+        <v>1282</v>
+      </c>
+      <c r="B1097" t="s">
+        <v>1295</v>
+      </c>
+      <c r="C1097" t="s">
+        <v>1299</v>
+      </c>
+      <c r="D1097" t="s">
+        <v>683</v>
+      </c>
+      <c r="E1097" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="1098" spans="1:5">
+      <c r="A1098" t="s">
+        <v>1282</v>
+      </c>
+      <c r="B1098" t="s">
+        <v>1296</v>
+      </c>
+      <c r="C1098" t="s">
+        <v>1299</v>
+      </c>
+      <c r="D1098" t="s">
+        <v>683</v>
+      </c>
+      <c r="E1098" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="1099" spans="1:5">
+      <c r="A1099" t="s">
+        <v>1282</v>
+      </c>
+      <c r="B1099" t="s">
+        <v>1297</v>
+      </c>
+      <c r="C1099" t="s">
+        <v>1299</v>
+      </c>
+      <c r="D1099" t="s">
+        <v>683</v>
+      </c>
+      <c r="E1099" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="1100" spans="1:5">
+      <c r="A1100" t="s">
+        <v>1282</v>
+      </c>
+      <c r="B1100" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C1100" t="s">
+        <v>1299</v>
+      </c>
+      <c r="D1100" t="s">
+        <v>683</v>
+      </c>
+      <c r="E1100" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="1101" spans="1:5">
+      <c r="A1101" t="s">
+        <v>1282</v>
+      </c>
+      <c r="B1101" t="s">
+        <v>1293</v>
+      </c>
+      <c r="C1101" t="s">
+        <v>1299</v>
+      </c>
+      <c r="D1101" t="s">
+        <v>683</v>
+      </c>
+      <c r="E1101" t="s">
+        <v>651</v>
       </c>
     </row>
   </sheetData>

</xml_diff>